<commit_message>
Finished planning in "Zeitplan" and worked on "IPA-Bericht"
</commit_message>
<xml_diff>
--- a/_Dokumente/Zeitplan.xlsx
+++ b/_Dokumente/Zeitplan.xlsx
@@ -1,9 +1,9 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23029"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23127"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AAC63D66-5FCB-421F-BE4A-0660A2A3ADBC}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E897F1D7-21C0-41A1-A574-564B27035A7A}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="25820" windowHeight="14620" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -477,7 +477,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="57">
+  <cellXfs count="59">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
@@ -547,48 +547,6 @@
     <xf numFmtId="164" fontId="4" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="2" borderId="2" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="3" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="3" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="3" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="1" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="49" fontId="3" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" textRotation="90"/>
-    </xf>
     <xf numFmtId="164" fontId="4" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="164" fontId="4" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="164" fontId="4" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1"/>
@@ -607,10 +565,25 @@
     <xf numFmtId="164" fontId="4" fillId="4" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="3" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="3" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="3" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="3" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -618,6 +591,39 @@
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="2" borderId="2" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="1" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="3" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="4" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -906,10 +912,16 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <sheetPr>
+    <pageSetUpPr fitToPage="1"/>
+  </sheetPr>
   <dimension ref="C2:CT66"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A19" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="T42" sqref="T42"/>
+    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <pane xSplit="3" ySplit="5" topLeftCell="D6" activePane="bottomRight" state="frozen"/>
+      <selection pane="topRight" activeCell="D1" sqref="D1"/>
+      <selection pane="bottomLeft" activeCell="A6" sqref="A6"/>
+      <selection pane="bottomRight" activeCell="AM22" sqref="AM22:AN22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.81640625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -925,13 +937,13 @@
       <c r="C2" s="6" t="s">
         <v>0</v>
       </c>
-      <c r="D2" s="42" t="s">
+      <c r="D2" s="44" t="s">
         <v>3</v>
       </c>
-      <c r="E2" s="42" t="s">
+      <c r="E2" s="44" t="s">
         <v>2</v>
       </c>
-      <c r="F2" s="42" t="s">
+      <c r="F2" s="44" t="s">
         <v>4</v>
       </c>
     </row>
@@ -939,347 +951,347 @@
       <c r="C3" s="4" t="s">
         <v>22</v>
       </c>
-      <c r="D3" s="42"/>
-      <c r="E3" s="42"/>
-      <c r="F3" s="42"/>
+      <c r="D3" s="44"/>
+      <c r="E3" s="44"/>
+      <c r="F3" s="44"/>
     </row>
     <row r="4" spans="3:98" x14ac:dyDescent="0.35">
       <c r="C4" s="4" t="s">
         <v>14</v>
       </c>
-      <c r="D4" s="42"/>
-      <c r="E4" s="42"/>
-      <c r="F4" s="42"/>
-      <c r="G4" s="34" t="s">
+      <c r="D4" s="44"/>
+      <c r="E4" s="44"/>
+      <c r="F4" s="44"/>
+      <c r="G4" s="41" t="s">
         <v>15</v>
       </c>
-      <c r="H4" s="34"/>
-      <c r="I4" s="34"/>
-      <c r="J4" s="35"/>
-      <c r="K4" s="41" t="s">
+      <c r="H4" s="41"/>
+      <c r="I4" s="41"/>
+      <c r="J4" s="42"/>
+      <c r="K4" s="39" t="s">
         <v>16</v>
       </c>
-      <c r="L4" s="41"/>
-      <c r="M4" s="41"/>
-      <c r="N4" s="41"/>
-      <c r="O4" s="41" t="s">
+      <c r="L4" s="39"/>
+      <c r="M4" s="39"/>
+      <c r="N4" s="39"/>
+      <c r="O4" s="39" t="s">
         <v>17</v>
       </c>
-      <c r="P4" s="41"/>
-      <c r="Q4" s="41"/>
-      <c r="R4" s="41"/>
-      <c r="S4" s="41" t="s">
+      <c r="P4" s="39"/>
+      <c r="Q4" s="39"/>
+      <c r="R4" s="39"/>
+      <c r="S4" s="39" t="s">
         <v>18</v>
       </c>
-      <c r="T4" s="41"/>
-      <c r="U4" s="41"/>
-      <c r="V4" s="41"/>
-      <c r="W4" s="41" t="s">
+      <c r="T4" s="39"/>
+      <c r="U4" s="39"/>
+      <c r="V4" s="39"/>
+      <c r="W4" s="39" t="s">
         <v>19</v>
       </c>
-      <c r="X4" s="41"/>
-      <c r="Y4" s="41"/>
-      <c r="Z4" s="41"/>
-      <c r="AA4" s="41" t="s">
+      <c r="X4" s="39"/>
+      <c r="Y4" s="39"/>
+      <c r="Z4" s="39"/>
+      <c r="AA4" s="39" t="s">
         <v>20</v>
       </c>
-      <c r="AB4" s="41"/>
-      <c r="AC4" s="41"/>
-      <c r="AD4" s="41"/>
-      <c r="AE4" s="41" t="s">
+      <c r="AB4" s="39"/>
+      <c r="AC4" s="39"/>
+      <c r="AD4" s="39"/>
+      <c r="AE4" s="39" t="s">
         <v>21</v>
       </c>
-      <c r="AF4" s="41"/>
-      <c r="AG4" s="41"/>
-      <c r="AH4" s="41"/>
-      <c r="AI4" s="33" t="s">
+      <c r="AF4" s="39"/>
+      <c r="AG4" s="39"/>
+      <c r="AH4" s="39"/>
+      <c r="AI4" s="40" t="s">
         <v>24</v>
       </c>
-      <c r="AJ4" s="34"/>
-      <c r="AK4" s="34"/>
-      <c r="AL4" s="35"/>
-      <c r="AM4" s="33" t="s">
+      <c r="AJ4" s="41"/>
+      <c r="AK4" s="41"/>
+      <c r="AL4" s="42"/>
+      <c r="AM4" s="40" t="s">
         <v>25</v>
       </c>
-      <c r="AN4" s="34"/>
-      <c r="AO4" s="34"/>
-      <c r="AP4" s="35"/>
-      <c r="AQ4" s="33" t="s">
+      <c r="AN4" s="41"/>
+      <c r="AO4" s="41"/>
+      <c r="AP4" s="42"/>
+      <c r="AQ4" s="40" t="s">
         <v>26</v>
       </c>
-      <c r="AR4" s="34"/>
-      <c r="AS4" s="34"/>
-      <c r="AT4" s="35"/>
-      <c r="AU4" s="33" t="s">
+      <c r="AR4" s="41"/>
+      <c r="AS4" s="41"/>
+      <c r="AT4" s="42"/>
+      <c r="AU4" s="40" t="s">
         <v>27</v>
       </c>
-      <c r="AV4" s="34"/>
-      <c r="AW4" s="34"/>
-      <c r="AX4" s="35"/>
-      <c r="AY4" s="33" t="s">
+      <c r="AV4" s="41"/>
+      <c r="AW4" s="41"/>
+      <c r="AX4" s="42"/>
+      <c r="AY4" s="40" t="s">
         <v>28</v>
       </c>
-      <c r="AZ4" s="34"/>
-      <c r="BA4" s="34"/>
-      <c r="BB4" s="35"/>
-      <c r="BC4" s="33" t="s">
+      <c r="AZ4" s="41"/>
+      <c r="BA4" s="41"/>
+      <c r="BB4" s="42"/>
+      <c r="BC4" s="40" t="s">
         <v>29</v>
       </c>
-      <c r="BD4" s="34"/>
-      <c r="BE4" s="34"/>
-      <c r="BF4" s="35"/>
-      <c r="BG4" s="33" t="s">
+      <c r="BD4" s="41"/>
+      <c r="BE4" s="41"/>
+      <c r="BF4" s="42"/>
+      <c r="BG4" s="40" t="s">
         <v>30</v>
       </c>
-      <c r="BH4" s="34"/>
-      <c r="BI4" s="34"/>
-      <c r="BJ4" s="35"/>
-      <c r="BK4" s="33" t="s">
+      <c r="BH4" s="41"/>
+      <c r="BI4" s="41"/>
+      <c r="BJ4" s="42"/>
+      <c r="BK4" s="40" t="s">
         <v>32</v>
       </c>
-      <c r="BL4" s="34"/>
-      <c r="BM4" s="34"/>
-      <c r="BN4" s="35"/>
-      <c r="BO4" s="33" t="s">
+      <c r="BL4" s="41"/>
+      <c r="BM4" s="41"/>
+      <c r="BN4" s="42"/>
+      <c r="BO4" s="40" t="s">
         <v>33</v>
       </c>
-      <c r="BP4" s="34"/>
-      <c r="BQ4" s="34"/>
-      <c r="BR4" s="35"/>
-      <c r="BS4" s="33" t="s">
+      <c r="BP4" s="41"/>
+      <c r="BQ4" s="41"/>
+      <c r="BR4" s="42"/>
+      <c r="BS4" s="40" t="s">
         <v>34</v>
       </c>
-      <c r="BT4" s="34"/>
-      <c r="BU4" s="34"/>
-      <c r="BV4" s="35"/>
-      <c r="BW4" s="33" t="s">
+      <c r="BT4" s="41"/>
+      <c r="BU4" s="41"/>
+      <c r="BV4" s="42"/>
+      <c r="BW4" s="40" t="s">
         <v>31</v>
       </c>
-      <c r="BX4" s="34"/>
-      <c r="BY4" s="34"/>
-      <c r="BZ4" s="35"/>
-      <c r="CA4" s="33" t="s">
+      <c r="BX4" s="41"/>
+      <c r="BY4" s="41"/>
+      <c r="BZ4" s="42"/>
+      <c r="CA4" s="40" t="s">
         <v>23</v>
       </c>
-      <c r="CB4" s="34"/>
-      <c r="CC4" s="34"/>
-      <c r="CD4" s="35"/>
-      <c r="CE4" s="33" t="s">
+      <c r="CB4" s="41"/>
+      <c r="CC4" s="41"/>
+      <c r="CD4" s="42"/>
+      <c r="CE4" s="40" t="s">
         <v>37</v>
       </c>
-      <c r="CF4" s="34"/>
-      <c r="CG4" s="34"/>
-      <c r="CH4" s="35"/>
-      <c r="CI4" s="33" t="s">
+      <c r="CF4" s="41"/>
+      <c r="CG4" s="41"/>
+      <c r="CH4" s="42"/>
+      <c r="CI4" s="40" t="s">
         <v>38</v>
       </c>
-      <c r="CJ4" s="34"/>
-      <c r="CK4" s="34"/>
-      <c r="CL4" s="35"/>
-      <c r="CM4" s="41" t="s">
+      <c r="CJ4" s="41"/>
+      <c r="CK4" s="41"/>
+      <c r="CL4" s="42"/>
+      <c r="CM4" s="39" t="s">
         <v>39</v>
       </c>
-      <c r="CN4" s="41"/>
-      <c r="CO4" s="41"/>
-      <c r="CP4" s="41"/>
-      <c r="CQ4" s="41" t="s">
+      <c r="CN4" s="39"/>
+      <c r="CO4" s="39"/>
+      <c r="CP4" s="39"/>
+      <c r="CQ4" s="39" t="s">
         <v>40</v>
       </c>
-      <c r="CR4" s="41"/>
-      <c r="CS4" s="41"/>
-      <c r="CT4" s="41"/>
+      <c r="CR4" s="39"/>
+      <c r="CS4" s="39"/>
+      <c r="CT4" s="39"/>
     </row>
     <row r="5" spans="3:98" x14ac:dyDescent="0.35">
       <c r="C5" s="5" t="s">
         <v>1</v>
       </c>
-      <c r="D5" s="42"/>
-      <c r="E5" s="42"/>
-      <c r="F5" s="42"/>
-      <c r="G5" s="53" t="s">
+      <c r="D5" s="44"/>
+      <c r="E5" s="44"/>
+      <c r="F5" s="44"/>
+      <c r="G5" s="45" t="s">
         <v>35</v>
       </c>
-      <c r="H5" s="54"/>
-      <c r="I5" s="54" t="s">
+      <c r="H5" s="43"/>
+      <c r="I5" s="43" t="s">
         <v>36</v>
       </c>
-      <c r="J5" s="54"/>
-      <c r="K5" s="54" t="s">
+      <c r="J5" s="43"/>
+      <c r="K5" s="43" t="s">
         <v>35</v>
       </c>
-      <c r="L5" s="54"/>
-      <c r="M5" s="54" t="s">
+      <c r="L5" s="43"/>
+      <c r="M5" s="43" t="s">
         <v>36</v>
       </c>
-      <c r="N5" s="54"/>
-      <c r="O5" s="54" t="s">
+      <c r="N5" s="43"/>
+      <c r="O5" s="43" t="s">
         <v>35</v>
       </c>
-      <c r="P5" s="54"/>
-      <c r="Q5" s="54" t="s">
+      <c r="P5" s="43"/>
+      <c r="Q5" s="43" t="s">
         <v>36</v>
       </c>
-      <c r="R5" s="54"/>
-      <c r="S5" s="54" t="s">
+      <c r="R5" s="43"/>
+      <c r="S5" s="43" t="s">
         <v>35</v>
       </c>
-      <c r="T5" s="54"/>
-      <c r="U5" s="54" t="s">
+      <c r="T5" s="43"/>
+      <c r="U5" s="43" t="s">
         <v>36</v>
       </c>
-      <c r="V5" s="54"/>
-      <c r="W5" s="54" t="s">
+      <c r="V5" s="43"/>
+      <c r="W5" s="43" t="s">
         <v>35</v>
       </c>
-      <c r="X5" s="54"/>
-      <c r="Y5" s="54" t="s">
+      <c r="X5" s="43"/>
+      <c r="Y5" s="43" t="s">
         <v>36</v>
       </c>
-      <c r="Z5" s="54"/>
-      <c r="AA5" s="54" t="s">
+      <c r="Z5" s="43"/>
+      <c r="AA5" s="43" t="s">
         <v>35</v>
       </c>
-      <c r="AB5" s="54"/>
-      <c r="AC5" s="54" t="s">
+      <c r="AB5" s="43"/>
+      <c r="AC5" s="43" t="s">
         <v>36</v>
       </c>
-      <c r="AD5" s="54"/>
-      <c r="AE5" s="54" t="s">
+      <c r="AD5" s="43"/>
+      <c r="AE5" s="43" t="s">
         <v>35</v>
       </c>
-      <c r="AF5" s="54"/>
-      <c r="AG5" s="54" t="s">
+      <c r="AF5" s="43"/>
+      <c r="AG5" s="43" t="s">
         <v>36</v>
       </c>
-      <c r="AH5" s="54"/>
-      <c r="AI5" s="55" t="s">
+      <c r="AH5" s="43"/>
+      <c r="AI5" s="46" t="s">
         <v>35</v>
       </c>
-      <c r="AJ5" s="56"/>
-      <c r="AK5" s="55" t="s">
+      <c r="AJ5" s="47"/>
+      <c r="AK5" s="46" t="s">
         <v>36</v>
       </c>
-      <c r="AL5" s="56"/>
-      <c r="AM5" s="55" t="s">
+      <c r="AL5" s="47"/>
+      <c r="AM5" s="46" t="s">
         <v>35</v>
       </c>
-      <c r="AN5" s="56"/>
-      <c r="AO5" s="55" t="s">
+      <c r="AN5" s="47"/>
+      <c r="AO5" s="46" t="s">
         <v>36</v>
       </c>
-      <c r="AP5" s="56"/>
-      <c r="AQ5" s="55" t="s">
+      <c r="AP5" s="47"/>
+      <c r="AQ5" s="46" t="s">
         <v>35</v>
       </c>
-      <c r="AR5" s="56"/>
-      <c r="AS5" s="55" t="s">
+      <c r="AR5" s="47"/>
+      <c r="AS5" s="46" t="s">
         <v>36</v>
       </c>
-      <c r="AT5" s="56"/>
-      <c r="AU5" s="55" t="s">
+      <c r="AT5" s="47"/>
+      <c r="AU5" s="46" t="s">
         <v>35</v>
       </c>
-      <c r="AV5" s="56"/>
-      <c r="AW5" s="55" t="s">
+      <c r="AV5" s="47"/>
+      <c r="AW5" s="46" t="s">
         <v>36</v>
       </c>
-      <c r="AX5" s="56"/>
-      <c r="AY5" s="55" t="s">
+      <c r="AX5" s="47"/>
+      <c r="AY5" s="46" t="s">
         <v>35</v>
       </c>
-      <c r="AZ5" s="56"/>
-      <c r="BA5" s="55" t="s">
+      <c r="AZ5" s="47"/>
+      <c r="BA5" s="46" t="s">
         <v>36</v>
       </c>
-      <c r="BB5" s="56"/>
-      <c r="BC5" s="55" t="s">
+      <c r="BB5" s="47"/>
+      <c r="BC5" s="46" t="s">
         <v>35</v>
       </c>
-      <c r="BD5" s="56"/>
-      <c r="BE5" s="55" t="s">
+      <c r="BD5" s="47"/>
+      <c r="BE5" s="46" t="s">
         <v>36</v>
       </c>
-      <c r="BF5" s="56"/>
-      <c r="BG5" s="55" t="s">
+      <c r="BF5" s="47"/>
+      <c r="BG5" s="46" t="s">
         <v>35</v>
       </c>
-      <c r="BH5" s="56"/>
-      <c r="BI5" s="55" t="s">
+      <c r="BH5" s="47"/>
+      <c r="BI5" s="46" t="s">
         <v>36</v>
       </c>
-      <c r="BJ5" s="56"/>
-      <c r="BK5" s="55" t="s">
+      <c r="BJ5" s="47"/>
+      <c r="BK5" s="46" t="s">
         <v>35</v>
       </c>
-      <c r="BL5" s="56"/>
-      <c r="BM5" s="55" t="s">
+      <c r="BL5" s="47"/>
+      <c r="BM5" s="46" t="s">
         <v>36</v>
       </c>
-      <c r="BN5" s="56"/>
-      <c r="BO5" s="55" t="s">
+      <c r="BN5" s="47"/>
+      <c r="BO5" s="46" t="s">
         <v>35</v>
       </c>
-      <c r="BP5" s="56"/>
-      <c r="BQ5" s="55" t="s">
+      <c r="BP5" s="47"/>
+      <c r="BQ5" s="46" t="s">
         <v>36</v>
       </c>
-      <c r="BR5" s="56"/>
-      <c r="BS5" s="55" t="s">
+      <c r="BR5" s="47"/>
+      <c r="BS5" s="46" t="s">
         <v>35</v>
       </c>
-      <c r="BT5" s="56"/>
-      <c r="BU5" s="55" t="s">
+      <c r="BT5" s="47"/>
+      <c r="BU5" s="46" t="s">
         <v>36</v>
       </c>
-      <c r="BV5" s="56"/>
-      <c r="BW5" s="55" t="s">
+      <c r="BV5" s="47"/>
+      <c r="BW5" s="46" t="s">
         <v>35</v>
       </c>
-      <c r="BX5" s="56"/>
-      <c r="BY5" s="55" t="s">
+      <c r="BX5" s="47"/>
+      <c r="BY5" s="46" t="s">
         <v>36</v>
       </c>
-      <c r="BZ5" s="56"/>
-      <c r="CA5" s="55" t="s">
+      <c r="BZ5" s="47"/>
+      <c r="CA5" s="46" t="s">
         <v>35</v>
       </c>
-      <c r="CB5" s="56"/>
-      <c r="CC5" s="55" t="s">
+      <c r="CB5" s="47"/>
+      <c r="CC5" s="46" t="s">
         <v>36</v>
       </c>
-      <c r="CD5" s="56"/>
-      <c r="CE5" s="55" t="s">
+      <c r="CD5" s="47"/>
+      <c r="CE5" s="46" t="s">
         <v>35</v>
       </c>
-      <c r="CF5" s="56"/>
-      <c r="CG5" s="55" t="s">
+      <c r="CF5" s="47"/>
+      <c r="CG5" s="46" t="s">
         <v>36</v>
       </c>
-      <c r="CH5" s="56"/>
-      <c r="CI5" s="55" t="s">
+      <c r="CH5" s="47"/>
+      <c r="CI5" s="46" t="s">
         <v>35</v>
       </c>
-      <c r="CJ5" s="56"/>
-      <c r="CK5" s="55" t="s">
+      <c r="CJ5" s="47"/>
+      <c r="CK5" s="46" t="s">
         <v>36</v>
       </c>
-      <c r="CL5" s="56"/>
-      <c r="CM5" s="54" t="s">
+      <c r="CL5" s="47"/>
+      <c r="CM5" s="43" t="s">
         <v>35</v>
       </c>
-      <c r="CN5" s="54"/>
-      <c r="CO5" s="54" t="s">
+      <c r="CN5" s="43"/>
+      <c r="CO5" s="43" t="s">
         <v>36</v>
       </c>
-      <c r="CP5" s="54"/>
-      <c r="CQ5" s="54" t="s">
+      <c r="CP5" s="43"/>
+      <c r="CQ5" s="43" t="s">
         <v>35</v>
       </c>
-      <c r="CR5" s="54"/>
-      <c r="CS5" s="54" t="s">
+      <c r="CR5" s="43"/>
+      <c r="CS5" s="43" t="s">
         <v>36</v>
       </c>
-      <c r="CT5" s="54"/>
+      <c r="CT5" s="43"/>
     </row>
     <row r="6" spans="3:98" x14ac:dyDescent="0.35">
       <c r="C6" s="1" t="s">
@@ -1382,25 +1394,25 @@
       <c r="CT6" s="3"/>
     </row>
     <row r="7" spans="3:98" ht="10.15" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="C7" s="29" t="s">
+      <c r="C7" s="48" t="s">
         <v>50</v>
       </c>
-      <c r="D7" s="30">
+      <c r="D7" s="49">
         <f t="shared" ref="D7:D9" si="0">SUM(G7:CT7)</f>
         <v>1.5</v>
       </c>
-      <c r="E7" s="30">
+      <c r="E7" s="49">
         <f t="shared" ref="E7:E9" si="1">SUM(G8:CT8)</f>
         <v>1.5</v>
       </c>
-      <c r="F7" s="30">
+      <c r="F7" s="49">
         <f>SUM($D$7:D7)-SUM($E$7:E7)</f>
         <v>0</v>
       </c>
-      <c r="G7" s="49">
+      <c r="G7" s="35">
         <v>1.5</v>
       </c>
-      <c r="H7" s="50"/>
+      <c r="H7" s="36"/>
       <c r="I7" s="21"/>
       <c r="J7" s="22"/>
       <c r="K7" s="11"/>
@@ -1493,14 +1505,14 @@
       <c r="CT7" s="10"/>
     </row>
     <row r="8" spans="3:98" ht="10.15" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="C8" s="29"/>
-      <c r="D8" s="31"/>
-      <c r="E8" s="31"/>
-      <c r="F8" s="31"/>
-      <c r="G8" s="51">
+      <c r="C8" s="48"/>
+      <c r="D8" s="50"/>
+      <c r="E8" s="50"/>
+      <c r="F8" s="50"/>
+      <c r="G8" s="37">
         <v>1.5</v>
       </c>
-      <c r="H8" s="52"/>
+      <c r="H8" s="38"/>
       <c r="I8" s="24"/>
       <c r="J8" s="25"/>
       <c r="K8" s="14"/>
@@ -1593,31 +1605,31 @@
       <c r="CT8" s="13"/>
     </row>
     <row r="9" spans="3:98" ht="10.15" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="C9" s="29" t="s">
+      <c r="C9" s="48" t="s">
         <v>41</v>
       </c>
-      <c r="D9" s="30">
+      <c r="D9" s="49">
         <f t="shared" si="0"/>
         <v>4.5</v>
       </c>
-      <c r="E9" s="30">
+      <c r="E9" s="49">
         <f t="shared" si="1"/>
         <v>4.5</v>
       </c>
-      <c r="F9" s="30">
+      <c r="F9" s="49">
         <f>SUM($D$7:D9)-SUM($E$7:E9)</f>
         <v>0</v>
       </c>
-      <c r="G9" s="49">
+      <c r="G9" s="35">
         <v>3</v>
       </c>
-      <c r="H9" s="50"/>
+      <c r="H9" s="36"/>
       <c r="I9" s="27"/>
       <c r="J9" s="28"/>
-      <c r="K9" s="49">
+      <c r="K9" s="35">
         <v>1.5</v>
       </c>
-      <c r="L9" s="50"/>
+      <c r="L9" s="36"/>
       <c r="M9" s="15"/>
       <c r="N9" s="16"/>
       <c r="O9" s="17"/>
@@ -1706,20 +1718,20 @@
       <c r="CT9" s="16"/>
     </row>
     <row r="10" spans="3:98" ht="10.15" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="C10" s="29"/>
-      <c r="D10" s="31"/>
-      <c r="E10" s="31"/>
-      <c r="F10" s="31"/>
-      <c r="G10" s="51">
+      <c r="C10" s="48"/>
+      <c r="D10" s="50"/>
+      <c r="E10" s="50"/>
+      <c r="F10" s="50"/>
+      <c r="G10" s="37">
         <v>3</v>
       </c>
-      <c r="H10" s="52"/>
+      <c r="H10" s="38"/>
       <c r="I10" s="24"/>
       <c r="J10" s="25"/>
-      <c r="K10" s="51">
+      <c r="K10" s="37">
         <v>1.5</v>
       </c>
-      <c r="L10" s="52"/>
+      <c r="L10" s="38"/>
       <c r="M10" s="12"/>
       <c r="N10" s="13"/>
       <c r="O10" s="14"/>
@@ -1808,18 +1820,18 @@
       <c r="CT10" s="13"/>
     </row>
     <row r="11" spans="3:98" ht="10.15" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="C11" s="29" t="s">
+      <c r="C11" s="48" t="s">
         <v>42</v>
       </c>
-      <c r="D11" s="30">
+      <c r="D11" s="49">
         <f t="shared" ref="D11" si="2">SUM(G11:CT11)</f>
         <v>7.5</v>
       </c>
-      <c r="E11" s="30">
+      <c r="E11" s="49">
         <f t="shared" ref="E11" si="3">SUM(G12:CT12)</f>
         <v>7.5</v>
       </c>
-      <c r="F11" s="30">
+      <c r="F11" s="49">
         <f>SUM($D$7:D11)-SUM($E$7:E11)</f>
         <v>0</v>
       </c>
@@ -1827,16 +1839,16 @@
       <c r="H11" s="27"/>
       <c r="I11" s="27"/>
       <c r="J11" s="28"/>
-      <c r="K11" s="49">
+      <c r="K11" s="35">
         <v>3</v>
       </c>
-      <c r="L11" s="50"/>
+      <c r="L11" s="36"/>
       <c r="M11" s="15"/>
       <c r="N11" s="16"/>
-      <c r="O11" s="49">
+      <c r="O11" s="35">
         <v>4.5</v>
       </c>
-      <c r="P11" s="50"/>
+      <c r="P11" s="36"/>
       <c r="Q11" s="15"/>
       <c r="R11" s="16"/>
       <c r="S11" s="17"/>
@@ -1921,24 +1933,24 @@
       <c r="CT11" s="16"/>
     </row>
     <row r="12" spans="3:98" ht="10.15" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="C12" s="29"/>
-      <c r="D12" s="31"/>
-      <c r="E12" s="31"/>
-      <c r="F12" s="31"/>
+      <c r="C12" s="48"/>
+      <c r="D12" s="50"/>
+      <c r="E12" s="50"/>
+      <c r="F12" s="50"/>
       <c r="G12" s="23"/>
       <c r="H12" s="24"/>
       <c r="I12" s="24"/>
       <c r="J12" s="25"/>
-      <c r="K12" s="51">
+      <c r="K12" s="37">
         <v>3</v>
       </c>
-      <c r="L12" s="52"/>
+      <c r="L12" s="38"/>
       <c r="M12" s="12"/>
       <c r="N12" s="13"/>
-      <c r="O12" s="51">
+      <c r="O12" s="37">
         <v>4.5</v>
       </c>
-      <c r="P12" s="52"/>
+      <c r="P12" s="38"/>
       <c r="Q12" s="12"/>
       <c r="R12" s="13"/>
       <c r="S12" s="14"/>
@@ -2023,18 +2035,18 @@
       <c r="CT12" s="13"/>
     </row>
     <row r="13" spans="3:98" ht="10.15" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="C13" s="29" t="s">
+      <c r="C13" s="48" t="s">
         <v>45</v>
       </c>
-      <c r="D13" s="30">
+      <c r="D13" s="49">
         <f t="shared" ref="D13" si="4">SUM(G13:CT13)</f>
         <v>3</v>
       </c>
-      <c r="E13" s="30">
+      <c r="E13" s="49">
         <f t="shared" ref="E13" si="5">SUM(G14:CT14)</f>
         <v>3</v>
       </c>
-      <c r="F13" s="30">
+      <c r="F13" s="49">
         <f>SUM($D$7:D13)-SUM($E$7:E13)</f>
         <v>0</v>
       </c>
@@ -2050,16 +2062,16 @@
       <c r="P13" s="15"/>
       <c r="Q13" s="15"/>
       <c r="R13" s="16"/>
-      <c r="S13" s="49">
+      <c r="S13" s="35">
         <v>1.5</v>
       </c>
-      <c r="T13" s="50"/>
+      <c r="T13" s="36"/>
       <c r="U13" s="15"/>
       <c r="V13" s="16"/>
-      <c r="W13" s="49">
+      <c r="W13" s="35">
         <v>1.5</v>
       </c>
-      <c r="X13" s="50"/>
+      <c r="X13" s="36"/>
       <c r="Y13" s="15"/>
       <c r="Z13" s="16"/>
       <c r="AA13" s="17"/>
@@ -2136,10 +2148,10 @@
       <c r="CT13" s="16"/>
     </row>
     <row r="14" spans="3:98" ht="10.15" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="C14" s="29"/>
-      <c r="D14" s="31"/>
-      <c r="E14" s="31"/>
-      <c r="F14" s="31"/>
+      <c r="C14" s="48"/>
+      <c r="D14" s="50"/>
+      <c r="E14" s="50"/>
+      <c r="F14" s="50"/>
       <c r="G14" s="23"/>
       <c r="H14" s="24"/>
       <c r="I14" s="24"/>
@@ -2152,16 +2164,16 @@
       <c r="P14" s="12"/>
       <c r="Q14" s="12"/>
       <c r="R14" s="13"/>
-      <c r="S14" s="51">
+      <c r="S14" s="37">
         <v>1.5</v>
       </c>
-      <c r="T14" s="52"/>
+      <c r="T14" s="38"/>
       <c r="U14" s="12"/>
       <c r="V14" s="13"/>
-      <c r="W14" s="51">
+      <c r="W14" s="37">
         <v>1.5</v>
       </c>
-      <c r="X14" s="52"/>
+      <c r="X14" s="38"/>
       <c r="Y14" s="12"/>
       <c r="Z14" s="13"/>
       <c r="AA14" s="14"/>
@@ -2238,18 +2250,18 @@
       <c r="CT14" s="13"/>
     </row>
     <row r="15" spans="3:98" ht="10.15" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="C15" s="29" t="s">
+      <c r="C15" s="48" t="s">
         <v>43</v>
       </c>
-      <c r="D15" s="30">
+      <c r="D15" s="49">
         <f t="shared" ref="D15" si="6">SUM(G15:CT15)</f>
         <v>3</v>
       </c>
-      <c r="E15" s="30">
+      <c r="E15" s="49">
         <f t="shared" ref="E15" si="7">SUM(G16:CT16)</f>
         <v>3</v>
       </c>
-      <c r="F15" s="30">
+      <c r="F15" s="49">
         <f>SUM($D$7:D15)-SUM($E$7:E15)</f>
         <v>0</v>
       </c>
@@ -2273,16 +2285,16 @@
       <c r="X15" s="15"/>
       <c r="Y15" s="15"/>
       <c r="Z15" s="16"/>
-      <c r="AA15" s="49">
+      <c r="AA15" s="35">
         <v>1.5</v>
       </c>
-      <c r="AB15" s="50"/>
+      <c r="AB15" s="36"/>
       <c r="AC15" s="15"/>
       <c r="AD15" s="16"/>
-      <c r="AE15" s="49">
+      <c r="AE15" s="35">
         <v>1.5</v>
       </c>
-      <c r="AF15" s="50"/>
+      <c r="AF15" s="36"/>
       <c r="AG15" s="15"/>
       <c r="AH15" s="16"/>
       <c r="AI15" s="17"/>
@@ -2351,10 +2363,10 @@
       <c r="CT15" s="16"/>
     </row>
     <row r="16" spans="3:98" ht="10.15" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="C16" s="29"/>
-      <c r="D16" s="31"/>
-      <c r="E16" s="31"/>
-      <c r="F16" s="31"/>
+      <c r="C16" s="48"/>
+      <c r="D16" s="50"/>
+      <c r="E16" s="50"/>
+      <c r="F16" s="50"/>
       <c r="G16" s="23"/>
       <c r="H16" s="24"/>
       <c r="I16" s="24"/>
@@ -2375,16 +2387,16 @@
       <c r="X16" s="12"/>
       <c r="Y16" s="12"/>
       <c r="Z16" s="13"/>
-      <c r="AA16" s="51">
+      <c r="AA16" s="37">
         <v>1.5</v>
       </c>
-      <c r="AB16" s="52"/>
+      <c r="AB16" s="38"/>
       <c r="AC16" s="12"/>
       <c r="AD16" s="13"/>
-      <c r="AE16" s="51">
+      <c r="AE16" s="37">
         <v>1.5</v>
       </c>
-      <c r="AF16" s="52"/>
+      <c r="AF16" s="38"/>
       <c r="AG16" s="12"/>
       <c r="AH16" s="13"/>
       <c r="AI16" s="14"/>
@@ -2453,20 +2465,20 @@
       <c r="CT16" s="13"/>
     </row>
     <row r="17" spans="3:98" ht="10.15" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="C17" s="29" t="s">
+      <c r="C17" s="48" t="s">
         <v>44</v>
       </c>
-      <c r="D17" s="30">
+      <c r="D17" s="49">
         <f t="shared" ref="D17" si="8">SUM(G17:CT17)</f>
         <v>1.5</v>
       </c>
-      <c r="E17" s="30">
+      <c r="E17" s="49">
         <f t="shared" ref="E17" si="9">SUM(G18:CT18)</f>
-        <v>1.5</v>
-      </c>
-      <c r="F17" s="30">
+        <v>2.5</v>
+      </c>
+      <c r="F17" s="49">
         <f>SUM($D$7:D17)-SUM($E$7:E17)</f>
-        <v>0</v>
+        <v>-1</v>
       </c>
       <c r="G17" s="26"/>
       <c r="H17" s="27"/>
@@ -2496,10 +2508,10 @@
       <c r="AF17" s="15"/>
       <c r="AG17" s="15"/>
       <c r="AH17" s="16"/>
-      <c r="AI17" s="49">
+      <c r="AI17" s="35">
         <v>1.5</v>
       </c>
-      <c r="AJ17" s="50"/>
+      <c r="AJ17" s="36"/>
       <c r="AK17" s="15"/>
       <c r="AL17" s="16"/>
       <c r="AM17" s="17"/>
@@ -2564,10 +2576,10 @@
       <c r="CT17" s="16"/>
     </row>
     <row r="18" spans="3:98" ht="10.15" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="C18" s="29"/>
-      <c r="D18" s="31"/>
-      <c r="E18" s="31"/>
-      <c r="F18" s="31"/>
+      <c r="C18" s="48"/>
+      <c r="D18" s="50"/>
+      <c r="E18" s="50"/>
+      <c r="F18" s="50"/>
       <c r="G18" s="20"/>
       <c r="H18" s="21"/>
       <c r="I18" s="21"/>
@@ -2596,14 +2608,16 @@
       <c r="AF18" s="9"/>
       <c r="AG18" s="9"/>
       <c r="AH18" s="10"/>
-      <c r="AI18" s="51">
+      <c r="AI18" s="37">
         <v>1.5</v>
       </c>
-      <c r="AJ18" s="52"/>
+      <c r="AJ18" s="38"/>
       <c r="AK18" s="9"/>
       <c r="AL18" s="10"/>
-      <c r="AM18" s="11"/>
-      <c r="AN18" s="9"/>
+      <c r="AM18" s="37">
+        <v>1</v>
+      </c>
+      <c r="AN18" s="38"/>
       <c r="AO18" s="9"/>
       <c r="AP18" s="10"/>
       <c r="AQ18" s="11"/>
@@ -2664,20 +2678,20 @@
       <c r="CT18" s="10"/>
     </row>
     <row r="19" spans="3:98" ht="10.15" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="C19" s="29" t="s">
+      <c r="C19" s="48" t="s">
         <v>46</v>
       </c>
-      <c r="D19" s="30">
+      <c r="D19" s="49">
         <f t="shared" ref="D19" si="10">SUM(G19:CT19)</f>
         <v>0.5</v>
       </c>
-      <c r="E19" s="30">
+      <c r="E19" s="49">
         <f t="shared" ref="E19" si="11">SUM(G20:CT20)</f>
-        <v>0</v>
-      </c>
-      <c r="F19" s="30">
+        <v>0.5</v>
+      </c>
+      <c r="F19" s="49">
         <f>SUM($D$7:D19)-SUM($E$7:E19)</f>
-        <v>0.5</v>
+        <v>-1</v>
       </c>
       <c r="G19" s="26"/>
       <c r="H19" s="27"/>
@@ -2707,14 +2721,14 @@
       <c r="AF19" s="15"/>
       <c r="AG19" s="15"/>
       <c r="AH19" s="16"/>
-      <c r="AI19" s="43"/>
-      <c r="AJ19" s="44"/>
+      <c r="AI19" s="29"/>
+      <c r="AJ19" s="30"/>
       <c r="AK19" s="15"/>
       <c r="AL19" s="16"/>
-      <c r="AM19" s="49">
+      <c r="AM19" s="35">
         <v>0.5</v>
       </c>
-      <c r="AN19" s="50"/>
+      <c r="AN19" s="36"/>
       <c r="AO19" s="15"/>
       <c r="AP19" s="16"/>
       <c r="AQ19" s="17"/>
@@ -2775,10 +2789,10 @@
       <c r="CT19" s="16"/>
     </row>
     <row r="20" spans="3:98" ht="10.15" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="C20" s="29"/>
-      <c r="D20" s="31"/>
-      <c r="E20" s="31"/>
-      <c r="F20" s="31"/>
+      <c r="C20" s="48"/>
+      <c r="D20" s="50"/>
+      <c r="E20" s="50"/>
+      <c r="F20" s="50"/>
       <c r="G20" s="20"/>
       <c r="H20" s="21"/>
       <c r="I20" s="21"/>
@@ -2807,12 +2821,14 @@
       <c r="AF20" s="9"/>
       <c r="AG20" s="9"/>
       <c r="AH20" s="10"/>
-      <c r="AI20" s="45"/>
-      <c r="AJ20" s="46"/>
+      <c r="AI20" s="31"/>
+      <c r="AJ20" s="32"/>
       <c r="AK20" s="9"/>
       <c r="AL20" s="10"/>
-      <c r="AM20" s="51"/>
-      <c r="AN20" s="52"/>
+      <c r="AM20" s="37">
+        <v>0.5</v>
+      </c>
+      <c r="AN20" s="38"/>
       <c r="AO20" s="9"/>
       <c r="AP20" s="10"/>
       <c r="AQ20" s="11"/>
@@ -2873,20 +2889,20 @@
       <c r="CT20" s="10"/>
     </row>
     <row r="21" spans="3:98" ht="10.15" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="C21" s="29" t="s">
+      <c r="C21" s="48" t="s">
         <v>47</v>
       </c>
-      <c r="D21" s="30">
+      <c r="D21" s="49">
         <f t="shared" ref="D21" si="12">SUM(G21:CT21)</f>
         <v>1</v>
       </c>
-      <c r="E21" s="30">
+      <c r="E21" s="49">
         <f t="shared" ref="E21" si="13">SUM(G22:CT22)</f>
         <v>0</v>
       </c>
-      <c r="F21" s="30">
+      <c r="F21" s="49">
         <f>SUM($D$7:D21)-SUM($E$7:E21)</f>
-        <v>1.5</v>
+        <v>0</v>
       </c>
       <c r="G21" s="26"/>
       <c r="H21" s="27"/>
@@ -2916,14 +2932,14 @@
       <c r="AF21" s="15"/>
       <c r="AG21" s="15"/>
       <c r="AH21" s="16"/>
-      <c r="AI21" s="43"/>
-      <c r="AJ21" s="44"/>
+      <c r="AI21" s="29"/>
+      <c r="AJ21" s="30"/>
       <c r="AK21" s="15"/>
       <c r="AL21" s="16"/>
-      <c r="AM21" s="49">
+      <c r="AM21" s="35">
         <v>1</v>
       </c>
-      <c r="AN21" s="50"/>
+      <c r="AN21" s="36"/>
       <c r="AO21" s="15"/>
       <c r="AP21" s="16"/>
       <c r="AQ21" s="17"/>
@@ -2984,10 +3000,10 @@
       <c r="CT21" s="16"/>
     </row>
     <row r="22" spans="3:98" ht="10.15" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="C22" s="29"/>
-      <c r="D22" s="31"/>
-      <c r="E22" s="31"/>
-      <c r="F22" s="31"/>
+      <c r="C22" s="48"/>
+      <c r="D22" s="50"/>
+      <c r="E22" s="50"/>
+      <c r="F22" s="50"/>
       <c r="G22" s="20"/>
       <c r="H22" s="21"/>
       <c r="I22" s="21"/>
@@ -3016,12 +3032,12 @@
       <c r="AF22" s="9"/>
       <c r="AG22" s="9"/>
       <c r="AH22" s="10"/>
-      <c r="AI22" s="45"/>
-      <c r="AJ22" s="46"/>
+      <c r="AI22" s="31"/>
+      <c r="AJ22" s="32"/>
       <c r="AK22" s="9"/>
       <c r="AL22" s="10"/>
-      <c r="AM22" s="51"/>
-      <c r="AN22" s="52"/>
+      <c r="AM22" s="37"/>
+      <c r="AN22" s="38"/>
       <c r="AO22" s="9"/>
       <c r="AP22" s="10"/>
       <c r="AQ22" s="11"/>
@@ -3082,20 +3098,20 @@
       <c r="CT22" s="10"/>
     </row>
     <row r="23" spans="3:98" ht="10.15" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="C23" s="29" t="s">
+      <c r="C23" s="48" t="s">
         <v>48</v>
       </c>
-      <c r="D23" s="30">
+      <c r="D23" s="49">
         <f t="shared" ref="D23" si="14">SUM(G23:CT23)</f>
         <v>0.5</v>
       </c>
-      <c r="E23" s="30">
+      <c r="E23" s="49">
         <f t="shared" ref="E23" si="15">SUM(G24:CT24)</f>
         <v>0</v>
       </c>
-      <c r="F23" s="30">
+      <c r="F23" s="49">
         <f>SUM($D$7:D23)-SUM($E$7:E23)</f>
-        <v>2</v>
+        <v>0.5</v>
       </c>
       <c r="G23" s="26"/>
       <c r="H23" s="27"/>
@@ -3125,18 +3141,18 @@
       <c r="AF23" s="15"/>
       <c r="AG23" s="15"/>
       <c r="AH23" s="16"/>
-      <c r="AI23" s="43"/>
-      <c r="AJ23" s="44"/>
+      <c r="AI23" s="29"/>
+      <c r="AJ23" s="30"/>
       <c r="AK23" s="15"/>
       <c r="AL23" s="16"/>
-      <c r="AM23" s="47"/>
-      <c r="AN23" s="48"/>
+      <c r="AM23" s="33"/>
+      <c r="AN23" s="34"/>
       <c r="AO23" s="15"/>
       <c r="AP23" s="16"/>
-      <c r="AQ23" s="49">
+      <c r="AQ23" s="35">
         <v>0.5</v>
       </c>
-      <c r="AR23" s="50"/>
+      <c r="AR23" s="36"/>
       <c r="AS23" s="15"/>
       <c r="AT23" s="16"/>
       <c r="AU23" s="17"/>
@@ -3193,10 +3209,10 @@
       <c r="CT23" s="16"/>
     </row>
     <row r="24" spans="3:98" ht="10.15" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="C24" s="29"/>
-      <c r="D24" s="31"/>
-      <c r="E24" s="31"/>
-      <c r="F24" s="31"/>
+      <c r="C24" s="48"/>
+      <c r="D24" s="50"/>
+      <c r="E24" s="50"/>
+      <c r="F24" s="50"/>
       <c r="G24" s="20"/>
       <c r="H24" s="21"/>
       <c r="I24" s="21"/>
@@ -3225,16 +3241,16 @@
       <c r="AF24" s="9"/>
       <c r="AG24" s="9"/>
       <c r="AH24" s="10"/>
-      <c r="AI24" s="45"/>
-      <c r="AJ24" s="46"/>
+      <c r="AI24" s="31"/>
+      <c r="AJ24" s="32"/>
       <c r="AK24" s="9"/>
       <c r="AL24" s="10"/>
-      <c r="AM24" s="45"/>
-      <c r="AN24" s="46"/>
+      <c r="AM24" s="31"/>
+      <c r="AN24" s="32"/>
       <c r="AO24" s="9"/>
       <c r="AP24" s="10"/>
-      <c r="AQ24" s="51"/>
-      <c r="AR24" s="52"/>
+      <c r="AQ24" s="37"/>
+      <c r="AR24" s="38"/>
       <c r="AS24" s="9"/>
       <c r="AT24" s="10"/>
       <c r="AU24" s="11"/>
@@ -3291,20 +3307,20 @@
       <c r="CT24" s="10"/>
     </row>
     <row r="25" spans="3:98" ht="10.15" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="C25" s="29" t="s">
+      <c r="C25" s="48" t="s">
         <v>49</v>
       </c>
-      <c r="D25" s="30">
+      <c r="D25" s="49">
         <f t="shared" ref="D25:D34" si="16">SUM(G25:CT25)</f>
         <v>1</v>
       </c>
-      <c r="E25" s="30">
+      <c r="E25" s="49">
         <f>SUM(G26:CT26)</f>
         <v>0</v>
       </c>
-      <c r="F25" s="30">
+      <c r="F25" s="49">
         <f>SUM($D$7:D25)-SUM($E$7:E25)</f>
-        <v>3</v>
+        <v>1.5</v>
       </c>
       <c r="G25" s="26"/>
       <c r="H25" s="27"/>
@@ -3334,18 +3350,18 @@
       <c r="AF25" s="15"/>
       <c r="AG25" s="15"/>
       <c r="AH25" s="16"/>
-      <c r="AI25" s="43"/>
-      <c r="AJ25" s="44"/>
+      <c r="AI25" s="29"/>
+      <c r="AJ25" s="30"/>
       <c r="AK25" s="15"/>
       <c r="AL25" s="16"/>
-      <c r="AM25" s="47"/>
-      <c r="AN25" s="48"/>
+      <c r="AM25" s="33"/>
+      <c r="AN25" s="34"/>
       <c r="AO25" s="15"/>
       <c r="AP25" s="16"/>
-      <c r="AQ25" s="49">
+      <c r="AQ25" s="35">
         <v>1</v>
       </c>
-      <c r="AR25" s="50"/>
+      <c r="AR25" s="36"/>
       <c r="AS25" s="15"/>
       <c r="AT25" s="16"/>
       <c r="AU25" s="17"/>
@@ -3402,10 +3418,10 @@
       <c r="CT25" s="16"/>
     </row>
     <row r="26" spans="3:98" ht="10.15" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="C26" s="29"/>
-      <c r="D26" s="31"/>
-      <c r="E26" s="31"/>
-      <c r="F26" s="31"/>
+      <c r="C26" s="48"/>
+      <c r="D26" s="50"/>
+      <c r="E26" s="50"/>
+      <c r="F26" s="50"/>
       <c r="G26" s="20"/>
       <c r="H26" s="21"/>
       <c r="I26" s="21"/>
@@ -3434,16 +3450,16 @@
       <c r="AF26" s="9"/>
       <c r="AG26" s="9"/>
       <c r="AH26" s="10"/>
-      <c r="AI26" s="45"/>
-      <c r="AJ26" s="46"/>
+      <c r="AI26" s="31"/>
+      <c r="AJ26" s="32"/>
       <c r="AK26" s="9"/>
       <c r="AL26" s="10"/>
-      <c r="AM26" s="45"/>
-      <c r="AN26" s="46"/>
+      <c r="AM26" s="31"/>
+      <c r="AN26" s="32"/>
       <c r="AO26" s="9"/>
       <c r="AP26" s="10"/>
-      <c r="AQ26" s="51"/>
-      <c r="AR26" s="52"/>
+      <c r="AQ26" s="37"/>
+      <c r="AR26" s="38"/>
       <c r="AS26" s="9"/>
       <c r="AT26" s="10"/>
       <c r="AU26" s="11"/>
@@ -3600,20 +3616,20 @@
       <c r="CT27" s="19"/>
     </row>
     <row r="28" spans="3:98" ht="10.15" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="C28" s="40" t="s">
+      <c r="C28" s="51" t="s">
         <v>51</v>
       </c>
-      <c r="D28" s="30">
+      <c r="D28" s="49">
         <f t="shared" si="16"/>
-        <v>0</v>
-      </c>
-      <c r="E28" s="30">
+        <v>0.5</v>
+      </c>
+      <c r="E28" s="49">
         <f t="shared" ref="E28:E34" si="17">SUM(G29:CT29)</f>
         <v>0</v>
       </c>
-      <c r="F28" s="30">
+      <c r="F28" s="49">
         <f>SUM($D$7:D28)-SUM($E$7:E28)</f>
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="G28" s="11"/>
       <c r="H28" s="9"/>
@@ -3655,8 +3671,10 @@
       <c r="AR28" s="9"/>
       <c r="AS28" s="9"/>
       <c r="AT28" s="10"/>
-      <c r="AU28" s="11"/>
-      <c r="AV28" s="9"/>
+      <c r="AU28" s="35">
+        <v>0.5</v>
+      </c>
+      <c r="AV28" s="36"/>
       <c r="AW28" s="9"/>
       <c r="AX28" s="10"/>
       <c r="AY28" s="11"/>
@@ -3709,10 +3727,10 @@
       <c r="CT28" s="10"/>
     </row>
     <row r="29" spans="3:98" ht="10.15" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="C29" s="40"/>
-      <c r="D29" s="31"/>
-      <c r="E29" s="31"/>
-      <c r="F29" s="31"/>
+      <c r="C29" s="51"/>
+      <c r="D29" s="50"/>
+      <c r="E29" s="50"/>
+      <c r="F29" s="50"/>
       <c r="G29" s="14"/>
       <c r="H29" s="12"/>
       <c r="I29" s="12"/>
@@ -3753,8 +3771,8 @@
       <c r="AR29" s="12"/>
       <c r="AS29" s="12"/>
       <c r="AT29" s="13"/>
-      <c r="AU29" s="14"/>
-      <c r="AV29" s="12"/>
+      <c r="AU29" s="37"/>
+      <c r="AV29" s="38"/>
       <c r="AW29" s="12"/>
       <c r="AX29" s="13"/>
       <c r="AY29" s="14"/>
@@ -3807,20 +3825,20 @@
       <c r="CT29" s="13"/>
     </row>
     <row r="30" spans="3:98" ht="10.15" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="C30" s="40" t="s">
+      <c r="C30" s="51" t="s">
         <v>52</v>
       </c>
-      <c r="D30" s="30">
+      <c r="D30" s="49">
         <f t="shared" si="16"/>
-        <v>0</v>
-      </c>
-      <c r="E30" s="30">
+        <v>0.5</v>
+      </c>
+      <c r="E30" s="49">
         <f t="shared" si="17"/>
         <v>0</v>
       </c>
-      <c r="F30" s="30">
+      <c r="F30" s="49">
         <f>SUM($D$7:D30)-SUM($E$7:E30)</f>
-        <v>3</v>
+        <v>2.5</v>
       </c>
       <c r="G30" s="17"/>
       <c r="H30" s="15"/>
@@ -3862,8 +3880,10 @@
       <c r="AR30" s="15"/>
       <c r="AS30" s="15"/>
       <c r="AT30" s="16"/>
-      <c r="AU30" s="17"/>
-      <c r="AV30" s="15"/>
+      <c r="AU30" s="35">
+        <v>0.5</v>
+      </c>
+      <c r="AV30" s="36"/>
       <c r="AW30" s="15"/>
       <c r="AX30" s="16"/>
       <c r="AY30" s="17"/>
@@ -3916,10 +3936,10 @@
       <c r="CT30" s="16"/>
     </row>
     <row r="31" spans="3:98" ht="10.15" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="C31" s="40"/>
-      <c r="D31" s="31"/>
-      <c r="E31" s="31"/>
-      <c r="F31" s="31"/>
+      <c r="C31" s="51"/>
+      <c r="D31" s="50"/>
+      <c r="E31" s="50"/>
+      <c r="F31" s="50"/>
       <c r="G31" s="14"/>
       <c r="H31" s="12"/>
       <c r="I31" s="12"/>
@@ -3960,8 +3980,8 @@
       <c r="AR31" s="12"/>
       <c r="AS31" s="12"/>
       <c r="AT31" s="13"/>
-      <c r="AU31" s="14"/>
-      <c r="AV31" s="12"/>
+      <c r="AU31" s="37"/>
+      <c r="AV31" s="38"/>
       <c r="AW31" s="12"/>
       <c r="AX31" s="13"/>
       <c r="AY31" s="14"/>
@@ -4014,18 +4034,18 @@
       <c r="CT31" s="13"/>
     </row>
     <row r="32" spans="3:98" ht="10.15" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="C32" s="40" t="s">
+      <c r="C32" s="51" t="s">
         <v>53</v>
       </c>
-      <c r="D32" s="30">
+      <c r="D32" s="49">
         <f t="shared" si="16"/>
-        <v>0</v>
-      </c>
-      <c r="E32" s="30">
+        <v>0.5</v>
+      </c>
+      <c r="E32" s="49">
         <f t="shared" si="17"/>
         <v>0</v>
       </c>
-      <c r="F32" s="30">
+      <c r="F32" s="49">
         <f>SUM($D$7:D32)-SUM($E$7:E32)</f>
         <v>3</v>
       </c>
@@ -4069,8 +4089,10 @@
       <c r="AR32" s="15"/>
       <c r="AS32" s="15"/>
       <c r="AT32" s="16"/>
-      <c r="AU32" s="17"/>
-      <c r="AV32" s="15"/>
+      <c r="AU32" s="35">
+        <v>0.5</v>
+      </c>
+      <c r="AV32" s="36"/>
       <c r="AW32" s="15"/>
       <c r="AX32" s="16"/>
       <c r="AY32" s="17"/>
@@ -4123,10 +4145,10 @@
       <c r="CT32" s="16"/>
     </row>
     <row r="33" spans="3:98" ht="10.15" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="C33" s="40"/>
-      <c r="D33" s="31"/>
-      <c r="E33" s="31"/>
-      <c r="F33" s="31"/>
+      <c r="C33" s="51"/>
+      <c r="D33" s="50"/>
+      <c r="E33" s="50"/>
+      <c r="F33" s="50"/>
       <c r="G33" s="14"/>
       <c r="H33" s="12"/>
       <c r="I33" s="12"/>
@@ -4167,8 +4189,8 @@
       <c r="AR33" s="12"/>
       <c r="AS33" s="12"/>
       <c r="AT33" s="13"/>
-      <c r="AU33" s="14"/>
-      <c r="AV33" s="12"/>
+      <c r="AU33" s="37"/>
+      <c r="AV33" s="38"/>
       <c r="AW33" s="12"/>
       <c r="AX33" s="13"/>
       <c r="AY33" s="14"/>
@@ -4221,20 +4243,20 @@
       <c r="CT33" s="13"/>
     </row>
     <row r="34" spans="3:98" ht="10.15" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="C34" s="40" t="s">
+      <c r="C34" s="51" t="s">
         <v>54</v>
       </c>
-      <c r="D34" s="30">
+      <c r="D34" s="49">
         <f t="shared" si="16"/>
-        <v>0</v>
-      </c>
-      <c r="E34" s="30">
+        <v>1</v>
+      </c>
+      <c r="E34" s="49">
         <f t="shared" si="17"/>
         <v>0</v>
       </c>
-      <c r="F34" s="30">
+      <c r="F34" s="49">
         <f>SUM($D$7:D34)-SUM($E$7:E34)</f>
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="G34" s="17"/>
       <c r="H34" s="15"/>
@@ -4280,8 +4302,10 @@
       <c r="AV34" s="15"/>
       <c r="AW34" s="15"/>
       <c r="AX34" s="16"/>
-      <c r="AY34" s="17"/>
-      <c r="AZ34" s="15"/>
+      <c r="AY34" s="35">
+        <v>1</v>
+      </c>
+      <c r="AZ34" s="36"/>
       <c r="BA34" s="15"/>
       <c r="BB34" s="16"/>
       <c r="BC34" s="17"/>
@@ -4330,10 +4354,10 @@
       <c r="CT34" s="16"/>
     </row>
     <row r="35" spans="3:98" ht="10.15" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="C35" s="40"/>
-      <c r="D35" s="31"/>
-      <c r="E35" s="31"/>
-      <c r="F35" s="31"/>
+      <c r="C35" s="51"/>
+      <c r="D35" s="50"/>
+      <c r="E35" s="50"/>
+      <c r="F35" s="50"/>
       <c r="G35" s="14"/>
       <c r="H35" s="12"/>
       <c r="I35" s="12"/>
@@ -4378,8 +4402,8 @@
       <c r="AV35" s="12"/>
       <c r="AW35" s="12"/>
       <c r="AX35" s="13"/>
-      <c r="AY35" s="14"/>
-      <c r="AZ35" s="12"/>
+      <c r="AY35" s="37"/>
+      <c r="AZ35" s="38"/>
       <c r="BA35" s="12"/>
       <c r="BB35" s="13"/>
       <c r="BC35" s="14"/>
@@ -4528,20 +4552,20 @@
       <c r="CT36" s="19"/>
     </row>
     <row r="37" spans="3:98" ht="10.15" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="C37" s="29" t="s">
+      <c r="C37" s="48" t="s">
         <v>55</v>
       </c>
-      <c r="D37" s="30">
+      <c r="D37" s="49">
         <f t="shared" ref="D37:D59" si="18">SUM(G37:CT37)</f>
-        <v>0</v>
-      </c>
-      <c r="E37" s="30">
+        <v>0.5</v>
+      </c>
+      <c r="E37" s="49">
         <f t="shared" ref="E37:E59" si="19">SUM(G38:CT38)</f>
         <v>0</v>
       </c>
-      <c r="F37" s="30">
+      <c r="F37" s="49">
         <f>SUM($D$7:D37)-SUM($E$7:E37)</f>
-        <v>3</v>
+        <v>4.5</v>
       </c>
       <c r="G37" s="11"/>
       <c r="H37" s="9"/>
@@ -4587,8 +4611,10 @@
       <c r="AV37" s="21"/>
       <c r="AW37" s="21"/>
       <c r="AX37" s="22"/>
-      <c r="AY37" s="20"/>
-      <c r="AZ37" s="21"/>
+      <c r="AY37" s="35">
+        <v>0.5</v>
+      </c>
+      <c r="AZ37" s="36"/>
       <c r="BA37" s="21"/>
       <c r="BB37" s="22"/>
       <c r="BC37" s="20"/>
@@ -4637,10 +4663,10 @@
       <c r="CT37" s="22"/>
     </row>
     <row r="38" spans="3:98" ht="10.15" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="C38" s="29"/>
-      <c r="D38" s="31"/>
-      <c r="E38" s="31"/>
-      <c r="F38" s="31"/>
+      <c r="C38" s="48"/>
+      <c r="D38" s="50"/>
+      <c r="E38" s="50"/>
+      <c r="F38" s="50"/>
       <c r="G38" s="14"/>
       <c r="H38" s="12"/>
       <c r="I38" s="12"/>
@@ -4685,8 +4711,8 @@
       <c r="AV38" s="24"/>
       <c r="AW38" s="24"/>
       <c r="AX38" s="25"/>
-      <c r="AY38" s="23"/>
-      <c r="AZ38" s="24"/>
+      <c r="AY38" s="37"/>
+      <c r="AZ38" s="38"/>
       <c r="BA38" s="24"/>
       <c r="BB38" s="25"/>
       <c r="BC38" s="23"/>
@@ -4735,20 +4761,20 @@
       <c r="CT38" s="25"/>
     </row>
     <row r="39" spans="3:98" ht="10.15" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="C39" s="29" t="s">
+      <c r="C39" s="48" t="s">
         <v>57</v>
       </c>
-      <c r="D39" s="30">
+      <c r="D39" s="49">
         <f t="shared" si="18"/>
-        <v>0</v>
-      </c>
-      <c r="E39" s="30">
+        <v>0.5</v>
+      </c>
+      <c r="E39" s="49">
         <f t="shared" si="19"/>
         <v>0</v>
       </c>
-      <c r="F39" s="30">
+      <c r="F39" s="49">
         <f>SUM($D$7:D39)-SUM($E$7:E39)</f>
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="G39" s="17"/>
       <c r="H39" s="15"/>
@@ -4798,8 +4824,10 @@
       <c r="AZ39" s="27"/>
       <c r="BA39" s="27"/>
       <c r="BB39" s="28"/>
-      <c r="BC39" s="26"/>
-      <c r="BD39" s="27"/>
+      <c r="BC39" s="35">
+        <v>0.5</v>
+      </c>
+      <c r="BD39" s="36"/>
       <c r="BE39" s="27"/>
       <c r="BF39" s="28"/>
       <c r="BG39" s="26"/>
@@ -4844,10 +4872,10 @@
       <c r="CT39" s="28"/>
     </row>
     <row r="40" spans="3:98" ht="10.15" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="C40" s="29"/>
-      <c r="D40" s="31"/>
-      <c r="E40" s="31"/>
-      <c r="F40" s="31"/>
+      <c r="C40" s="48"/>
+      <c r="D40" s="50"/>
+      <c r="E40" s="50"/>
+      <c r="F40" s="50"/>
       <c r="G40" s="14"/>
       <c r="H40" s="12"/>
       <c r="I40" s="12"/>
@@ -4896,8 +4924,8 @@
       <c r="AZ40" s="24"/>
       <c r="BA40" s="24"/>
       <c r="BB40" s="25"/>
-      <c r="BC40" s="23"/>
-      <c r="BD40" s="24"/>
+      <c r="BC40" s="37"/>
+      <c r="BD40" s="38"/>
       <c r="BE40" s="24"/>
       <c r="BF40" s="25"/>
       <c r="BG40" s="23"/>
@@ -4942,20 +4970,20 @@
       <c r="CT40" s="25"/>
     </row>
     <row r="41" spans="3:98" ht="10.15" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="C41" s="29" t="s">
+      <c r="C41" s="48" t="s">
         <v>56</v>
       </c>
-      <c r="D41" s="30">
+      <c r="D41" s="49">
         <f t="shared" si="18"/>
-        <v>0</v>
-      </c>
-      <c r="E41" s="30">
+        <v>0.5</v>
+      </c>
+      <c r="E41" s="49">
         <f t="shared" si="19"/>
         <v>0</v>
       </c>
-      <c r="F41" s="30">
+      <c r="F41" s="49">
         <f>SUM($D$7:D41)-SUM($E$7:E41)</f>
-        <v>3</v>
+        <v>5.5</v>
       </c>
       <c r="G41" s="17"/>
       <c r="H41" s="15"/>
@@ -5005,8 +5033,10 @@
       <c r="AZ41" s="27"/>
       <c r="BA41" s="27"/>
       <c r="BB41" s="28"/>
-      <c r="BC41" s="26"/>
-      <c r="BD41" s="27"/>
+      <c r="BC41" s="35">
+        <v>0.5</v>
+      </c>
+      <c r="BD41" s="36"/>
       <c r="BE41" s="27"/>
       <c r="BF41" s="28"/>
       <c r="BG41" s="26"/>
@@ -5051,10 +5081,10 @@
       <c r="CT41" s="28"/>
     </row>
     <row r="42" spans="3:98" ht="10.15" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="C42" s="29"/>
-      <c r="D42" s="31"/>
-      <c r="E42" s="31"/>
-      <c r="F42" s="31"/>
+      <c r="C42" s="48"/>
+      <c r="D42" s="50"/>
+      <c r="E42" s="50"/>
+      <c r="F42" s="50"/>
       <c r="G42" s="14"/>
       <c r="H42" s="12"/>
       <c r="I42" s="12"/>
@@ -5103,8 +5133,8 @@
       <c r="AZ42" s="24"/>
       <c r="BA42" s="24"/>
       <c r="BB42" s="25"/>
-      <c r="BC42" s="23"/>
-      <c r="BD42" s="24"/>
+      <c r="BC42" s="37"/>
+      <c r="BD42" s="38"/>
       <c r="BE42" s="24"/>
       <c r="BF42" s="25"/>
       <c r="BG42" s="23"/>
@@ -5149,20 +5179,20 @@
       <c r="CT42" s="25"/>
     </row>
     <row r="43" spans="3:98" ht="10.15" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="C43" s="29" t="s">
+      <c r="C43" s="48" t="s">
         <v>58</v>
       </c>
-      <c r="D43" s="30">
+      <c r="D43" s="49">
         <f t="shared" si="18"/>
-        <v>0</v>
-      </c>
-      <c r="E43" s="30">
+        <v>1.5</v>
+      </c>
+      <c r="E43" s="49">
         <f t="shared" si="19"/>
         <v>0</v>
       </c>
-      <c r="F43" s="30">
+      <c r="F43" s="49">
         <f>SUM($D$7:D43)-SUM($E$7:E43)</f>
-        <v>3</v>
+        <v>7</v>
       </c>
       <c r="G43" s="17"/>
       <c r="H43" s="15"/>
@@ -5212,10 +5242,14 @@
       <c r="AZ43" s="27"/>
       <c r="BA43" s="27"/>
       <c r="BB43" s="28"/>
-      <c r="BC43" s="26"/>
-      <c r="BD43" s="27"/>
-      <c r="BE43" s="27"/>
-      <c r="BF43" s="28"/>
+      <c r="BC43" s="35">
+        <v>0.5</v>
+      </c>
+      <c r="BD43" s="36"/>
+      <c r="BE43" s="36">
+        <v>1</v>
+      </c>
+      <c r="BF43" s="57"/>
       <c r="BG43" s="26"/>
       <c r="BH43" s="27"/>
       <c r="BI43" s="27"/>
@@ -5258,10 +5292,10 @@
       <c r="CT43" s="28"/>
     </row>
     <row r="44" spans="3:98" ht="10.15" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="C44" s="29"/>
-      <c r="D44" s="31"/>
-      <c r="E44" s="31"/>
-      <c r="F44" s="31"/>
+      <c r="C44" s="48"/>
+      <c r="D44" s="50"/>
+      <c r="E44" s="50"/>
+      <c r="F44" s="50"/>
       <c r="G44" s="14"/>
       <c r="H44" s="12"/>
       <c r="I44" s="12"/>
@@ -5310,10 +5344,10 @@
       <c r="AZ44" s="24"/>
       <c r="BA44" s="24"/>
       <c r="BB44" s="25"/>
-      <c r="BC44" s="23"/>
-      <c r="BD44" s="24"/>
-      <c r="BE44" s="24"/>
-      <c r="BF44" s="25"/>
+      <c r="BC44" s="37"/>
+      <c r="BD44" s="38"/>
+      <c r="BE44" s="38"/>
+      <c r="BF44" s="58"/>
       <c r="BG44" s="23"/>
       <c r="BH44" s="24"/>
       <c r="BI44" s="24"/>
@@ -5356,20 +5390,20 @@
       <c r="CT44" s="25"/>
     </row>
     <row r="45" spans="3:98" ht="10.15" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="C45" s="29" t="s">
+      <c r="C45" s="48" t="s">
         <v>59</v>
       </c>
-      <c r="D45" s="30">
+      <c r="D45" s="49">
         <f t="shared" si="18"/>
-        <v>0</v>
-      </c>
-      <c r="E45" s="30">
+        <v>1.5</v>
+      </c>
+      <c r="E45" s="49">
         <f t="shared" si="19"/>
         <v>0</v>
       </c>
-      <c r="F45" s="30">
+      <c r="F45" s="49">
         <f>SUM($D$7:D45)-SUM($E$7:E45)</f>
-        <v>3</v>
+        <v>8.5</v>
       </c>
       <c r="G45" s="17"/>
       <c r="H45" s="15"/>
@@ -5423,8 +5457,10 @@
       <c r="BD45" s="27"/>
       <c r="BE45" s="27"/>
       <c r="BF45" s="28"/>
-      <c r="BG45" s="26"/>
-      <c r="BH45" s="27"/>
+      <c r="BG45" s="35">
+        <v>1.5</v>
+      </c>
+      <c r="BH45" s="36"/>
       <c r="BI45" s="27"/>
       <c r="BJ45" s="28"/>
       <c r="BK45" s="26"/>
@@ -5465,10 +5501,10 @@
       <c r="CT45" s="28"/>
     </row>
     <row r="46" spans="3:98" ht="10.15" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="C46" s="29"/>
-      <c r="D46" s="31"/>
-      <c r="E46" s="31"/>
-      <c r="F46" s="31"/>
+      <c r="C46" s="48"/>
+      <c r="D46" s="50"/>
+      <c r="E46" s="50"/>
+      <c r="F46" s="50"/>
       <c r="G46" s="14"/>
       <c r="H46" s="12"/>
       <c r="I46" s="12"/>
@@ -5521,8 +5557,8 @@
       <c r="BD46" s="24"/>
       <c r="BE46" s="24"/>
       <c r="BF46" s="25"/>
-      <c r="BG46" s="23"/>
-      <c r="BH46" s="24"/>
+      <c r="BG46" s="37"/>
+      <c r="BH46" s="38"/>
       <c r="BI46" s="24"/>
       <c r="BJ46" s="25"/>
       <c r="BK46" s="23"/>
@@ -5563,20 +5599,20 @@
       <c r="CT46" s="25"/>
     </row>
     <row r="47" spans="3:98" ht="10.15" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="C47" s="29" t="s">
+      <c r="C47" s="48" t="s">
         <v>60</v>
       </c>
-      <c r="D47" s="30">
+      <c r="D47" s="49">
         <f t="shared" si="18"/>
-        <v>0</v>
-      </c>
-      <c r="E47" s="30">
+        <v>2</v>
+      </c>
+      <c r="E47" s="49">
         <f t="shared" si="19"/>
         <v>0</v>
       </c>
-      <c r="F47" s="30">
+      <c r="F47" s="49">
         <f>SUM($D$7:D47)-SUM($E$7:E47)</f>
-        <v>3</v>
+        <v>10.5</v>
       </c>
       <c r="G47" s="17"/>
       <c r="H47" s="15"/>
@@ -5634,12 +5670,16 @@
       <c r="BH47" s="27"/>
       <c r="BI47" s="27"/>
       <c r="BJ47" s="28"/>
-      <c r="BK47" s="26"/>
-      <c r="BL47" s="27"/>
+      <c r="BK47" s="35">
+        <v>1.5</v>
+      </c>
+      <c r="BL47" s="36"/>
       <c r="BM47" s="27"/>
       <c r="BN47" s="28"/>
-      <c r="BO47" s="26"/>
-      <c r="BP47" s="27"/>
+      <c r="BO47" s="35">
+        <v>0.5</v>
+      </c>
+      <c r="BP47" s="36"/>
       <c r="BQ47" s="27"/>
       <c r="BR47" s="28"/>
       <c r="BS47" s="26"/>
@@ -5672,10 +5712,10 @@
       <c r="CT47" s="28"/>
     </row>
     <row r="48" spans="3:98" ht="10.15" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="C48" s="29"/>
-      <c r="D48" s="31"/>
-      <c r="E48" s="31"/>
-      <c r="F48" s="31"/>
+      <c r="C48" s="48"/>
+      <c r="D48" s="50"/>
+      <c r="E48" s="50"/>
+      <c r="F48" s="50"/>
       <c r="G48" s="14"/>
       <c r="H48" s="12"/>
       <c r="I48" s="12"/>
@@ -5732,12 +5772,12 @@
       <c r="BH48" s="24"/>
       <c r="BI48" s="24"/>
       <c r="BJ48" s="25"/>
-      <c r="BK48" s="23"/>
-      <c r="BL48" s="24"/>
+      <c r="BK48" s="37"/>
+      <c r="BL48" s="38"/>
       <c r="BM48" s="24"/>
       <c r="BN48" s="25"/>
-      <c r="BO48" s="23"/>
-      <c r="BP48" s="24"/>
+      <c r="BO48" s="37"/>
+      <c r="BP48" s="38"/>
       <c r="BQ48" s="24"/>
       <c r="BR48" s="25"/>
       <c r="BS48" s="23"/>
@@ -5770,20 +5810,20 @@
       <c r="CT48" s="25"/>
     </row>
     <row r="49" spans="3:98" ht="10.15" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="C49" s="29" t="s">
+      <c r="C49" s="48" t="s">
         <v>62</v>
       </c>
-      <c r="D49" s="30">
+      <c r="D49" s="49">
         <f t="shared" si="18"/>
-        <v>0</v>
-      </c>
-      <c r="E49" s="30">
+        <v>3</v>
+      </c>
+      <c r="E49" s="49">
         <f t="shared" si="19"/>
         <v>0</v>
       </c>
-      <c r="F49" s="30">
+      <c r="F49" s="49">
         <f>SUM($D$7:D49)-SUM($E$7:E49)</f>
-        <v>3</v>
+        <v>13.5</v>
       </c>
       <c r="G49" s="17"/>
       <c r="H49" s="15"/>
@@ -5845,12 +5885,18 @@
       <c r="BL49" s="27"/>
       <c r="BM49" s="27"/>
       <c r="BN49" s="28"/>
-      <c r="BO49" s="26"/>
-      <c r="BP49" s="27"/>
-      <c r="BQ49" s="27"/>
-      <c r="BR49" s="28"/>
-      <c r="BS49" s="26"/>
-      <c r="BT49" s="27"/>
+      <c r="BO49" s="35">
+        <v>1</v>
+      </c>
+      <c r="BP49" s="36"/>
+      <c r="BQ49" s="36">
+        <v>1</v>
+      </c>
+      <c r="BR49" s="57"/>
+      <c r="BS49" s="35">
+        <v>1</v>
+      </c>
+      <c r="BT49" s="36"/>
       <c r="BU49" s="27"/>
       <c r="BV49" s="28"/>
       <c r="BW49" s="26"/>
@@ -5879,10 +5925,10 @@
       <c r="CT49" s="28"/>
     </row>
     <row r="50" spans="3:98" ht="10.15" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="C50" s="29"/>
-      <c r="D50" s="31"/>
-      <c r="E50" s="31"/>
-      <c r="F50" s="31"/>
+      <c r="C50" s="48"/>
+      <c r="D50" s="50"/>
+      <c r="E50" s="50"/>
+      <c r="F50" s="50"/>
       <c r="G50" s="14"/>
       <c r="H50" s="12"/>
       <c r="I50" s="12"/>
@@ -5943,12 +5989,12 @@
       <c r="BL50" s="24"/>
       <c r="BM50" s="24"/>
       <c r="BN50" s="25"/>
-      <c r="BO50" s="23"/>
-      <c r="BP50" s="24"/>
-      <c r="BQ50" s="24"/>
-      <c r="BR50" s="25"/>
-      <c r="BS50" s="23"/>
-      <c r="BT50" s="24"/>
+      <c r="BO50" s="37"/>
+      <c r="BP50" s="38"/>
+      <c r="BQ50" s="38"/>
+      <c r="BR50" s="58"/>
+      <c r="BS50" s="37"/>
+      <c r="BT50" s="38"/>
       <c r="BU50" s="24"/>
       <c r="BV50" s="25"/>
       <c r="BW50" s="23"/>
@@ -5977,20 +6023,20 @@
       <c r="CT50" s="25"/>
     </row>
     <row r="51" spans="3:98" ht="10.15" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="C51" s="29" t="s">
+      <c r="C51" s="48" t="s">
         <v>63</v>
       </c>
-      <c r="D51" s="30">
+      <c r="D51" s="49">
         <f t="shared" si="18"/>
-        <v>0</v>
-      </c>
-      <c r="E51" s="30">
+        <v>3</v>
+      </c>
+      <c r="E51" s="49">
         <f t="shared" si="19"/>
         <v>0</v>
       </c>
-      <c r="F51" s="30">
+      <c r="F51" s="49">
         <f>SUM($D$7:D51)-SUM($E$7:E51)</f>
-        <v>3</v>
+        <v>16.5</v>
       </c>
       <c r="G51" s="17"/>
       <c r="H51" s="15"/>
@@ -6056,12 +6102,18 @@
       <c r="BP51" s="27"/>
       <c r="BQ51" s="27"/>
       <c r="BR51" s="28"/>
-      <c r="BS51" s="26"/>
-      <c r="BT51" s="27"/>
-      <c r="BU51" s="27"/>
-      <c r="BV51" s="28"/>
-      <c r="BW51" s="26"/>
-      <c r="BX51" s="27"/>
+      <c r="BS51" s="35">
+        <v>0.5</v>
+      </c>
+      <c r="BT51" s="36"/>
+      <c r="BU51" s="36">
+        <v>1</v>
+      </c>
+      <c r="BV51" s="57"/>
+      <c r="BW51" s="35">
+        <v>1.5</v>
+      </c>
+      <c r="BX51" s="36"/>
       <c r="BY51" s="27"/>
       <c r="BZ51" s="28"/>
       <c r="CA51" s="26"/>
@@ -6086,10 +6138,10 @@
       <c r="CT51" s="28"/>
     </row>
     <row r="52" spans="3:98" ht="10.15" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="C52" s="29"/>
-      <c r="D52" s="31"/>
-      <c r="E52" s="31"/>
-      <c r="F52" s="31"/>
+      <c r="C52" s="48"/>
+      <c r="D52" s="50"/>
+      <c r="E52" s="50"/>
+      <c r="F52" s="50"/>
       <c r="G52" s="14"/>
       <c r="H52" s="12"/>
       <c r="I52" s="12"/>
@@ -6154,12 +6206,12 @@
       <c r="BP52" s="24"/>
       <c r="BQ52" s="24"/>
       <c r="BR52" s="25"/>
-      <c r="BS52" s="23"/>
-      <c r="BT52" s="24"/>
-      <c r="BU52" s="24"/>
-      <c r="BV52" s="25"/>
-      <c r="BW52" s="23"/>
-      <c r="BX52" s="24"/>
+      <c r="BS52" s="37"/>
+      <c r="BT52" s="38"/>
+      <c r="BU52" s="38"/>
+      <c r="BV52" s="58"/>
+      <c r="BW52" s="37"/>
+      <c r="BX52" s="38"/>
       <c r="BY52" s="24"/>
       <c r="BZ52" s="25"/>
       <c r="CA52" s="23"/>
@@ -6184,20 +6236,20 @@
       <c r="CT52" s="25"/>
     </row>
     <row r="53" spans="3:98" ht="10.15" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="C53" s="29" t="s">
+      <c r="C53" s="48" t="s">
         <v>64</v>
       </c>
-      <c r="D53" s="30">
+      <c r="D53" s="49">
         <f t="shared" si="18"/>
-        <v>0</v>
-      </c>
-      <c r="E53" s="30">
+        <v>3</v>
+      </c>
+      <c r="E53" s="49">
         <f t="shared" si="19"/>
         <v>0</v>
       </c>
-      <c r="F53" s="30">
+      <c r="F53" s="49">
         <f>SUM($D$7:D53)-SUM($E$7:E53)</f>
-        <v>3</v>
+        <v>19.5</v>
       </c>
       <c r="G53" s="17"/>
       <c r="H53" s="15"/>
@@ -6271,12 +6323,18 @@
       <c r="BX53" s="27"/>
       <c r="BY53" s="27"/>
       <c r="BZ53" s="28"/>
-      <c r="CA53" s="26"/>
-      <c r="CB53" s="27"/>
-      <c r="CC53" s="27"/>
-      <c r="CD53" s="28"/>
-      <c r="CE53" s="26"/>
-      <c r="CF53" s="27"/>
+      <c r="CA53" s="35">
+        <v>1.5</v>
+      </c>
+      <c r="CB53" s="36"/>
+      <c r="CC53" s="36">
+        <v>1</v>
+      </c>
+      <c r="CD53" s="57"/>
+      <c r="CE53" s="35">
+        <v>0.5</v>
+      </c>
+      <c r="CF53" s="36"/>
       <c r="CG53" s="27"/>
       <c r="CH53" s="28"/>
       <c r="CI53" s="26"/>
@@ -6293,10 +6351,10 @@
       <c r="CT53" s="28"/>
     </row>
     <row r="54" spans="3:98" ht="10.15" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="C54" s="29"/>
-      <c r="D54" s="31"/>
-      <c r="E54" s="31"/>
-      <c r="F54" s="31"/>
+      <c r="C54" s="48"/>
+      <c r="D54" s="50"/>
+      <c r="E54" s="50"/>
+      <c r="F54" s="50"/>
       <c r="G54" s="14"/>
       <c r="H54" s="12"/>
       <c r="I54" s="12"/>
@@ -6369,12 +6427,12 @@
       <c r="BX54" s="24"/>
       <c r="BY54" s="24"/>
       <c r="BZ54" s="25"/>
-      <c r="CA54" s="23"/>
-      <c r="CB54" s="24"/>
-      <c r="CC54" s="24"/>
-      <c r="CD54" s="25"/>
-      <c r="CE54" s="23"/>
-      <c r="CF54" s="24"/>
+      <c r="CA54" s="37"/>
+      <c r="CB54" s="38"/>
+      <c r="CC54" s="38"/>
+      <c r="CD54" s="58"/>
+      <c r="CE54" s="37"/>
+      <c r="CF54" s="38"/>
       <c r="CG54" s="24"/>
       <c r="CH54" s="25"/>
       <c r="CI54" s="23"/>
@@ -6391,20 +6449,20 @@
       <c r="CT54" s="25"/>
     </row>
     <row r="55" spans="3:98" ht="10.15" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="C55" s="29" t="s">
+      <c r="C55" s="48" t="s">
         <v>65</v>
       </c>
-      <c r="D55" s="30">
+      <c r="D55" s="49">
         <f t="shared" si="18"/>
-        <v>0</v>
-      </c>
-      <c r="E55" s="30">
+        <v>3.5</v>
+      </c>
+      <c r="E55" s="49">
         <f t="shared" si="19"/>
         <v>0</v>
       </c>
-      <c r="F55" s="30">
+      <c r="F55" s="49">
         <f>SUM($D$7:D55)-SUM($E$7:E55)</f>
-        <v>3</v>
+        <v>23</v>
       </c>
       <c r="G55" s="17"/>
       <c r="H55" s="15"/>
@@ -6482,12 +6540,18 @@
       <c r="CB55" s="27"/>
       <c r="CC55" s="27"/>
       <c r="CD55" s="28"/>
-      <c r="CE55" s="26"/>
-      <c r="CF55" s="27"/>
-      <c r="CG55" s="27"/>
-      <c r="CH55" s="28"/>
-      <c r="CI55" s="26"/>
-      <c r="CJ55" s="27"/>
+      <c r="CE55" s="35">
+        <v>1</v>
+      </c>
+      <c r="CF55" s="36"/>
+      <c r="CG55" s="36">
+        <v>1</v>
+      </c>
+      <c r="CH55" s="57"/>
+      <c r="CI55" s="35">
+        <v>1.5</v>
+      </c>
+      <c r="CJ55" s="36"/>
       <c r="CK55" s="27"/>
       <c r="CL55" s="28"/>
       <c r="CM55" s="26"/>
@@ -6500,10 +6564,10 @@
       <c r="CT55" s="28"/>
     </row>
     <row r="56" spans="3:98" ht="10.15" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="C56" s="29"/>
-      <c r="D56" s="31"/>
-      <c r="E56" s="31"/>
-      <c r="F56" s="31"/>
+      <c r="C56" s="48"/>
+      <c r="D56" s="50"/>
+      <c r="E56" s="50"/>
+      <c r="F56" s="50"/>
       <c r="G56" s="14"/>
       <c r="H56" s="12"/>
       <c r="I56" s="12"/>
@@ -6580,12 +6644,12 @@
       <c r="CB56" s="24"/>
       <c r="CC56" s="24"/>
       <c r="CD56" s="25"/>
-      <c r="CE56" s="23"/>
-      <c r="CF56" s="24"/>
-      <c r="CG56" s="24"/>
-      <c r="CH56" s="25"/>
-      <c r="CI56" s="23"/>
-      <c r="CJ56" s="24"/>
+      <c r="CE56" s="37"/>
+      <c r="CF56" s="38"/>
+      <c r="CG56" s="38"/>
+      <c r="CH56" s="58"/>
+      <c r="CI56" s="37"/>
+      <c r="CJ56" s="38"/>
       <c r="CK56" s="24"/>
       <c r="CL56" s="25"/>
       <c r="CM56" s="23"/>
@@ -6598,20 +6662,20 @@
       <c r="CT56" s="25"/>
     </row>
     <row r="57" spans="3:98" ht="10.15" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="C57" s="29" t="s">
+      <c r="C57" s="48" t="s">
         <v>8</v>
       </c>
-      <c r="D57" s="30">
+      <c r="D57" s="49">
         <f t="shared" si="18"/>
-        <v>0</v>
-      </c>
-      <c r="E57" s="30">
+        <v>2.5</v>
+      </c>
+      <c r="E57" s="49">
         <f t="shared" si="19"/>
         <v>0</v>
       </c>
-      <c r="F57" s="30">
+      <c r="F57" s="49">
         <f>SUM($D$7:D57)-SUM($E$7:E57)</f>
-        <v>3</v>
+        <v>25.5</v>
       </c>
       <c r="G57" s="17"/>
       <c r="H57" s="15"/>
@@ -6697,20 +6761,24 @@
       <c r="CJ57" s="27"/>
       <c r="CK57" s="27"/>
       <c r="CL57" s="28"/>
-      <c r="CM57" s="26"/>
-      <c r="CN57" s="27"/>
-      <c r="CO57" s="27"/>
-      <c r="CP57" s="28"/>
+      <c r="CM57" s="35">
+        <v>1.5</v>
+      </c>
+      <c r="CN57" s="36"/>
+      <c r="CO57" s="36">
+        <v>1</v>
+      </c>
+      <c r="CP57" s="57"/>
       <c r="CQ57" s="26"/>
       <c r="CR57" s="27"/>
       <c r="CS57" s="27"/>
       <c r="CT57" s="28"/>
     </row>
     <row r="58" spans="3:98" ht="10.15" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="C58" s="29"/>
-      <c r="D58" s="31"/>
-      <c r="E58" s="31"/>
-      <c r="F58" s="31"/>
+      <c r="C58" s="48"/>
+      <c r="D58" s="50"/>
+      <c r="E58" s="50"/>
+      <c r="F58" s="50"/>
       <c r="G58" s="14"/>
       <c r="H58" s="12"/>
       <c r="I58" s="12"/>
@@ -6795,30 +6863,30 @@
       <c r="CJ58" s="24"/>
       <c r="CK58" s="24"/>
       <c r="CL58" s="25"/>
-      <c r="CM58" s="23"/>
-      <c r="CN58" s="24"/>
-      <c r="CO58" s="24"/>
-      <c r="CP58" s="25"/>
+      <c r="CM58" s="37"/>
+      <c r="CN58" s="38"/>
+      <c r="CO58" s="38"/>
+      <c r="CP58" s="58"/>
       <c r="CQ58" s="23"/>
       <c r="CR58" s="24"/>
       <c r="CS58" s="24"/>
       <c r="CT58" s="25"/>
     </row>
     <row r="59" spans="3:98" ht="10.15" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="C59" s="29" t="s">
+      <c r="C59" s="48" t="s">
         <v>61</v>
       </c>
-      <c r="D59" s="30">
+      <c r="D59" s="49">
         <f t="shared" si="18"/>
-        <v>0</v>
-      </c>
-      <c r="E59" s="30">
+        <v>2</v>
+      </c>
+      <c r="E59" s="49">
         <f t="shared" si="19"/>
         <v>0</v>
       </c>
-      <c r="F59" s="30">
+      <c r="F59" s="49">
         <f>SUM($D$7:D59)-SUM($E$7:E59)</f>
-        <v>3</v>
+        <v>27.5</v>
       </c>
       <c r="G59" s="17"/>
       <c r="H59" s="15"/>
@@ -6906,18 +6974,22 @@
       <c r="CL59" s="28"/>
       <c r="CM59" s="26"/>
       <c r="CN59" s="27"/>
-      <c r="CO59" s="27"/>
-      <c r="CP59" s="28"/>
-      <c r="CQ59" s="26"/>
-      <c r="CR59" s="27"/>
+      <c r="CO59" s="36">
+        <v>0.5</v>
+      </c>
+      <c r="CP59" s="57"/>
+      <c r="CQ59" s="35">
+        <v>1.5</v>
+      </c>
+      <c r="CR59" s="36"/>
       <c r="CS59" s="27"/>
       <c r="CT59" s="28"/>
     </row>
     <row r="60" spans="3:98" ht="10.15" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="C60" s="29"/>
-      <c r="D60" s="31"/>
-      <c r="E60" s="31"/>
-      <c r="F60" s="31"/>
+      <c r="C60" s="48"/>
+      <c r="D60" s="50"/>
+      <c r="E60" s="50"/>
+      <c r="F60" s="50"/>
       <c r="G60" s="11"/>
       <c r="H60" s="9"/>
       <c r="I60" s="9"/>
@@ -7004,10 +7076,10 @@
       <c r="CL60" s="22"/>
       <c r="CM60" s="20"/>
       <c r="CN60" s="21"/>
-      <c r="CO60" s="21"/>
-      <c r="CP60" s="22"/>
-      <c r="CQ60" s="20"/>
-      <c r="CR60" s="21"/>
+      <c r="CO60" s="38"/>
+      <c r="CP60" s="58"/>
+      <c r="CQ60" s="37"/>
+      <c r="CR60" s="38"/>
       <c r="CS60" s="21"/>
       <c r="CT60" s="22"/>
     </row>
@@ -7122,171 +7194,171 @@
       </c>
       <c r="D64" s="7">
         <f>SUM(D7:D60)</f>
-        <v>24</v>
+        <v>50</v>
       </c>
       <c r="E64" s="7"/>
       <c r="F64" s="8"/>
-      <c r="G64" s="32">
+      <c r="G64" s="52">
         <f>SUM(G7:J7,G9:J9,G11:J11,G13:J13,G15:J15,G17:J17,G19:J19,G21:J21,G23:J23,G25:J25,G28:J28,G30:J30,G32:J32,G34:J34,G37:J37,G39:J39,G41:J41,G43:J43,G45:J45,G47:J47,G49:J49,G51:J51,G53:J53,G55:J55,G57:J57,G59:J59)</f>
         <v>4.5</v>
       </c>
-      <c r="H64" s="36"/>
-      <c r="I64" s="36"/>
-      <c r="J64" s="37"/>
-      <c r="K64" s="32">
+      <c r="H64" s="53"/>
+      <c r="I64" s="53"/>
+      <c r="J64" s="54"/>
+      <c r="K64" s="52">
         <f t="shared" ref="K64:K65" si="20">SUM(K7:N7,K9:N9,K11:N11,K13:N13,K15:N15,K17:N17,K19:N19,K21:N21,K23:N23,K25:N25,K28:N28,K30:N30,K32:N32,K34:N34,K37:N37,K39:N39,K41:N41,K43:N43,K45:N45,K47:N47,K49:N49,K51:N51,K53:N53,K55:N55,K57:N57,K59:N59)</f>
         <v>4.5</v>
       </c>
-      <c r="L64" s="36"/>
-      <c r="M64" s="36"/>
-      <c r="N64" s="37"/>
-      <c r="O64" s="32">
+      <c r="L64" s="53"/>
+      <c r="M64" s="53"/>
+      <c r="N64" s="54"/>
+      <c r="O64" s="52">
         <f t="shared" ref="O64:O65" si="21">SUM(O7:R7,O9:R9,O11:R11,O13:R13,O15:R15,O17:R17,O19:R19,O21:R21,O23:R23,O25:R25,O28:R28,O30:R30,O32:R32,O34:R34,O37:R37,O39:R39,O41:R41,O43:R43,O45:R45,O47:R47,O49:R49,O51:R51,O53:R53,O55:R55,O57:R57,O59:R59)</f>
         <v>4.5</v>
       </c>
-      <c r="P64" s="36"/>
-      <c r="Q64" s="36"/>
-      <c r="R64" s="37"/>
-      <c r="S64" s="32">
+      <c r="P64" s="53"/>
+      <c r="Q64" s="53"/>
+      <c r="R64" s="54"/>
+      <c r="S64" s="52">
         <f t="shared" ref="S64:S65" si="22">SUM(S7:V7,S9:V9,S11:V11,S13:V13,S15:V15,S17:V17,S19:V19,S21:V21,S23:V23,S25:V25,S28:V28,S30:V30,S32:V32,S34:V34,S37:V37,S39:V39,S41:V41,S43:V43,S45:V45,S47:V47,S49:V49,S51:V51,S53:V53,S55:V55,S57:V57,S59:V59)</f>
         <v>1.5</v>
       </c>
-      <c r="T64" s="36"/>
-      <c r="U64" s="36"/>
-      <c r="V64" s="37"/>
-      <c r="W64" s="32">
+      <c r="T64" s="53"/>
+      <c r="U64" s="53"/>
+      <c r="V64" s="54"/>
+      <c r="W64" s="52">
         <f t="shared" ref="W64:W65" si="23">SUM(W7:Z7,W9:Z9,W11:Z11,W13:Z13,W15:Z15,W17:Z17,W19:Z19,W21:Z21,W23:Z23,W25:Z25,W28:Z28,W30:Z30,W32:Z32,W34:Z34,W37:Z37,W39:Z39,W41:Z41,W43:Z43,W45:Z45,W47:Z47,W49:Z49,W51:Z51,W53:Z53,W55:Z55,W57:Z57,W59:Z59)</f>
         <v>1.5</v>
       </c>
-      <c r="X64" s="36"/>
-      <c r="Y64" s="36"/>
-      <c r="Z64" s="37"/>
-      <c r="AA64" s="32">
+      <c r="X64" s="53"/>
+      <c r="Y64" s="53"/>
+      <c r="Z64" s="54"/>
+      <c r="AA64" s="52">
         <f t="shared" ref="AA64:AA65" si="24">SUM(AA7:AD7,AA9:AD9,AA11:AD11,AA13:AD13,AA15:AD15,AA17:AD17,AA19:AD19,AA21:AD21,AA23:AD23,AA25:AD25,AA28:AD28,AA30:AD30,AA32:AD32,AA34:AD34,AA37:AD37,AA39:AD39,AA41:AD41,AA43:AD43,AA45:AD45,AA47:AD47,AA49:AD49,AA51:AD51,AA53:AD53,AA55:AD55,AA57:AD57,AA59:AD59)</f>
         <v>1.5</v>
       </c>
-      <c r="AB64" s="36"/>
-      <c r="AC64" s="36"/>
-      <c r="AD64" s="37"/>
-      <c r="AE64" s="32">
+      <c r="AB64" s="53"/>
+      <c r="AC64" s="53"/>
+      <c r="AD64" s="54"/>
+      <c r="AE64" s="52">
         <f t="shared" ref="AE64:AE65" si="25">SUM(AE7:AH7,AE9:AH9,AE11:AH11,AE13:AH13,AE15:AH15,AE17:AH17,AE19:AH19,AE21:AH21,AE23:AH23,AE25:AH25,AE28:AH28,AE30:AH30,AE32:AH32,AE34:AH34,AE37:AH37,AE39:AH39,AE41:AH41,AE43:AH43,AE45:AH45,AE47:AH47,AE49:AH49,AE51:AH51,AE53:AH53,AE55:AH55,AE57:AH57,AE59:AH59)</f>
         <v>1.5</v>
       </c>
-      <c r="AF64" s="36"/>
-      <c r="AG64" s="36"/>
-      <c r="AH64" s="37"/>
-      <c r="AI64" s="32">
+      <c r="AF64" s="53"/>
+      <c r="AG64" s="53"/>
+      <c r="AH64" s="54"/>
+      <c r="AI64" s="52">
         <f t="shared" ref="AI64:AI65" si="26">SUM(AI7:AL7,AI9:AL9,AI11:AL11,AI13:AL13,AI15:AL15,AI17:AL17,AI19:AL19,AI21:AL21,AI23:AL23,AI25:AL25,AI28:AL28,AI30:AL30,AI32:AL32,AI34:AL34,AI37:AL37,AI39:AL39,AI41:AL41,AI43:AL43,AI45:AL45,AI47:AL47,AI49:AL49,AI51:AL51,AI53:AL53,AI55:AL55,AI57:AL57,AI59:AL59)</f>
         <v>1.5</v>
       </c>
-      <c r="AJ64" s="36"/>
-      <c r="AK64" s="36"/>
-      <c r="AL64" s="37"/>
-      <c r="AM64" s="32">
+      <c r="AJ64" s="53"/>
+      <c r="AK64" s="53"/>
+      <c r="AL64" s="54"/>
+      <c r="AM64" s="52">
         <f t="shared" ref="AM64:AM65" si="27">SUM(AM7:AP7,AM9:AP9,AM11:AP11,AM13:AP13,AM15:AP15,AM17:AP17,AM19:AP19,AM21:AP21,AM23:AP23,AM25:AP25,AM28:AP28,AM30:AP30,AM32:AP32,AM34:AP34,AM37:AP37,AM39:AP39,AM41:AP41,AM43:AP43,AM45:AP45,AM47:AP47,AM49:AP49,AM51:AP51,AM53:AP53,AM55:AP55,AM57:AP57,AM59:AP59)</f>
         <v>1.5</v>
       </c>
-      <c r="AN64" s="36"/>
-      <c r="AO64" s="36"/>
-      <c r="AP64" s="37"/>
-      <c r="AQ64" s="32">
+      <c r="AN64" s="53"/>
+      <c r="AO64" s="53"/>
+      <c r="AP64" s="54"/>
+      <c r="AQ64" s="52">
         <f t="shared" ref="AQ64:AQ65" si="28">SUM(AQ7:AT7,AQ9:AT9,AQ11:AT11,AQ13:AT13,AQ15:AT15,AQ17:AT17,AQ19:AT19,AQ21:AT21,AQ23:AT23,AQ25:AT25,AQ28:AT28,AQ30:AT30,AQ32:AT32,AQ34:AT34,AQ37:AT37,AQ39:AT39,AQ41:AT41,AQ43:AT43,AQ45:AT45,AQ47:AT47,AQ49:AT49,AQ51:AT51,AQ53:AT53,AQ55:AT55,AQ57:AT57,AQ59:AT59)</f>
         <v>1.5</v>
       </c>
-      <c r="AR64" s="36"/>
-      <c r="AS64" s="36"/>
-      <c r="AT64" s="37"/>
-      <c r="AU64" s="32">
+      <c r="AR64" s="53"/>
+      <c r="AS64" s="53"/>
+      <c r="AT64" s="54"/>
+      <c r="AU64" s="52">
         <f t="shared" ref="AU64:AU65" si="29">SUM(AU7:AX7,AU9:AX9,AU11:AX11,AU13:AX13,AU15:AX15,AU17:AX17,AU19:AX19,AU21:AX21,AU23:AX23,AU25:AX25,AU28:AX28,AU30:AX30,AU32:AX32,AU34:AX34,AU37:AX37,AU39:AX39,AU41:AX41,AU43:AX43,AU45:AX45,AU47:AX47,AU49:AX49,AU51:AX51,AU53:AX53,AU55:AX55,AU57:AX57,AU59:AX59)</f>
-        <v>0</v>
-      </c>
-      <c r="AV64" s="36"/>
-      <c r="AW64" s="36"/>
-      <c r="AX64" s="37"/>
-      <c r="AY64" s="32">
+        <v>1.5</v>
+      </c>
+      <c r="AV64" s="53"/>
+      <c r="AW64" s="53"/>
+      <c r="AX64" s="54"/>
+      <c r="AY64" s="52">
         <f t="shared" ref="AY64:AY65" si="30">SUM(AY7:BB7,AY9:BB9,AY11:BB11,AY13:BB13,AY15:BB15,AY17:BB17,AY19:BB19,AY21:BB21,AY23:BB23,AY25:BB25,AY28:BB28,AY30:BB30,AY32:BB32,AY34:BB34,AY37:BB37,AY39:BB39,AY41:BB41,AY43:BB43,AY45:BB45,AY47:BB47,AY49:BB49,AY51:BB51,AY53:BB53,AY55:BB55,AY57:BB57,AY59:BB59)</f>
-        <v>0</v>
-      </c>
-      <c r="AZ64" s="36"/>
-      <c r="BA64" s="36"/>
-      <c r="BB64" s="37"/>
-      <c r="BC64" s="32">
+        <v>1.5</v>
+      </c>
+      <c r="AZ64" s="53"/>
+      <c r="BA64" s="53"/>
+      <c r="BB64" s="54"/>
+      <c r="BC64" s="52">
         <f t="shared" ref="BC64:BC65" si="31">SUM(BC7:BF7,BC9:BF9,BC11:BF11,BC13:BF13,BC15:BF15,BC17:BF17,BC19:BF19,BC21:BF21,BC23:BF23,BC25:BF25,BC28:BF28,BC30:BF30,BC32:BF32,BC34:BF34,BC37:BF37,BC39:BF39,BC41:BF41,BC43:BF43,BC45:BF45,BC47:BF47,BC49:BF49,BC51:BF51,BC53:BF53,BC55:BF55,BC57:BF57,BC59:BF59)</f>
-        <v>0</v>
-      </c>
-      <c r="BD64" s="36"/>
-      <c r="BE64" s="36"/>
-      <c r="BF64" s="37"/>
-      <c r="BG64" s="32">
+        <v>2.5</v>
+      </c>
+      <c r="BD64" s="53"/>
+      <c r="BE64" s="53"/>
+      <c r="BF64" s="54"/>
+      <c r="BG64" s="52">
         <f t="shared" ref="BG64:BG65" si="32">SUM(BG7:BJ7,BG9:BJ9,BG11:BJ11,BG13:BJ13,BG15:BJ15,BG17:BJ17,BG19:BJ19,BG21:BJ21,BG23:BJ23,BG25:BJ25,BG28:BJ28,BG30:BJ30,BG32:BJ32,BG34:BJ34,BG37:BJ37,BG39:BJ39,BG41:BJ41,BG43:BJ43,BG45:BJ45,BG47:BJ47,BG49:BJ49,BG51:BJ51,BG53:BJ53,BG55:BJ55,BG57:BJ57,BG59:BJ59)</f>
-        <v>0</v>
-      </c>
-      <c r="BH64" s="36"/>
-      <c r="BI64" s="36"/>
-      <c r="BJ64" s="37"/>
-      <c r="BK64" s="32">
+        <v>1.5</v>
+      </c>
+      <c r="BH64" s="53"/>
+      <c r="BI64" s="53"/>
+      <c r="BJ64" s="54"/>
+      <c r="BK64" s="52">
         <f t="shared" ref="BK64:BK65" si="33">SUM(BK7:BN7,BK9:BN9,BK11:BN11,BK13:BN13,BK15:BN15,BK17:BN17,BK19:BN19,BK21:BN21,BK23:BN23,BK25:BN25,BK28:BN28,BK30:BN30,BK32:BN32,BK34:BN34,BK37:BN37,BK39:BN39,BK41:BN41,BK43:BN43,BK45:BN45,BK47:BN47,BK49:BN49,BK51:BN51,BK53:BN53,BK55:BN55,BK57:BN57,BK59:BN59)</f>
-        <v>0</v>
-      </c>
-      <c r="BL64" s="36"/>
-      <c r="BM64" s="36"/>
-      <c r="BN64" s="37"/>
-      <c r="BO64" s="32">
-        <f t="shared" ref="BO64:BO65" si="34">SUM(BO7:BR7,BO9:BR9,BO11:BR11,BO13:BR13,BO15:BR15,BO17:BR17,BO19:BR19,BO21:BR21,BO23:BR23,BO25:BR25,BO28:BR28,BO30:BR30,BO32:BR32,BO34:BR34,BO37:BR37,BO39:BR39,BO41:BR41,BO43:BR43,BO45:BR45,BO47:BR47,BO49:BR49,BO51:BR51,BO53:BR53,BO55:BR55,BO57:BR57,BO59:BR59)</f>
-        <v>0</v>
-      </c>
-      <c r="BP64" s="36"/>
-      <c r="BQ64" s="36"/>
-      <c r="BR64" s="37"/>
-      <c r="BS64" s="32">
-        <f t="shared" ref="BS64:BS65" si="35">SUM(BS7:BV7,BS9:BV9,BS11:BV11,BS13:BV13,BS15:BV15,BS17:BV17,BS19:BV19,BS21:BV21,BS23:BV23,BS25:BV25,BS28:BV28,BS30:BV30,BS32:BV32,BS34:BV34,BS37:BV37,BS39:BV39,BS41:BV41,BS43:BV43,BS45:BV45,BS47:BV47,BS49:BV49,BS51:BV51,BS53:BV53,BS55:BV55,BS57:BV57,BS59:BV59)</f>
-        <v>0</v>
-      </c>
-      <c r="BT64" s="36"/>
-      <c r="BU64" s="36"/>
-      <c r="BV64" s="37"/>
-      <c r="BW64" s="32">
-        <f t="shared" ref="BW64:BW65" si="36">SUM(BW7:BZ7,BW9:BZ9,BW11:BZ11,BW13:BZ13,BW15:BZ15,BW17:BZ17,BW19:BZ19,BW21:BZ21,BW23:BZ23,BW25:BZ25,BW28:BZ28,BW30:BZ30,BW32:BZ32,BW34:BZ34,BW37:BZ37,BW39:BZ39,BW41:BZ41,BW43:BZ43,BW45:BZ45,BW47:BZ47,BW49:BZ49,BW51:BZ51,BW53:BZ53,BW55:BZ55,BW57:BZ57,BW59:BZ59)</f>
-        <v>0</v>
-      </c>
-      <c r="BX64" s="36"/>
-      <c r="BY64" s="36"/>
-      <c r="BZ64" s="37"/>
-      <c r="CA64" s="32">
-        <f t="shared" ref="CA64:CA65" si="37">SUM(CA7:CD7,CA9:CD9,CA11:CD11,CA13:CD13,CA15:CD15,CA17:CD17,CA19:CD19,CA21:CD21,CA23:CD23,CA25:CD25,CA28:CD28,CA30:CD30,CA32:CD32,CA34:CD34,CA37:CD37,CA39:CD39,CA41:CD41,CA43:CD43,CA45:CD45,CA47:CD47,CA49:CD49,CA51:CD51,CA53:CD53,CA55:CD55,CA57:CD57,CA59:CD59)</f>
-        <v>0</v>
-      </c>
-      <c r="CB64" s="36"/>
-      <c r="CC64" s="36"/>
-      <c r="CD64" s="37"/>
-      <c r="CE64" s="32">
-        <f t="shared" ref="CE64:CE65" si="38">SUM(CE7:CH7,CE9:CH9,CE11:CH11,CE13:CH13,CE15:CH15,CE17:CH17,CE19:CH19,CE21:CH21,CE23:CH23,CE25:CH25,CE28:CH28,CE30:CH30,CE32:CH32,CE34:CH34,CE37:CH37,CE39:CH39,CE41:CH41,CE43:CH43,CE45:CH45,CE47:CH47,CE49:CH49,CE51:CH51,CE53:CH53,CE55:CH55,CE57:CH57,CE59:CH59)</f>
-        <v>0</v>
-      </c>
-      <c r="CF64" s="36"/>
-      <c r="CG64" s="36"/>
-      <c r="CH64" s="37"/>
-      <c r="CI64" s="32">
-        <f t="shared" ref="CI64:CI65" si="39">SUM(CI7:CL7,CI9:CL9,CI11:CL11,CI13:CL13,CI15:CL15,CI17:CL17,CI19:CL19,CI21:CL21,CI23:CL23,CI25:CL25,CI28:CL28,CI30:CL30,CI32:CL32,CI34:CL34,CI37:CL37,CI39:CL39,CI41:CL41,CI43:CL43,CI45:CL45,CI47:CL47,CI49:CL49,CI51:CL51,CI53:CL53,CI55:CL55,CI57:CL57,CI59:CL59)</f>
-        <v>0</v>
-      </c>
-      <c r="CJ64" s="36"/>
-      <c r="CK64" s="36"/>
-      <c r="CL64" s="37"/>
-      <c r="CM64" s="32">
-        <f t="shared" ref="CM64:CM65" si="40">SUM(CM7:CP7,CM9:CP9,CM11:CP11,CM13:CP13,CM15:CP15,CM17:CP17,CM19:CP19,CM21:CP21,CM23:CP23,CM25:CP25,CM28:CP28,CM30:CP30,CM32:CP32,CM34:CP34,CM37:CP37,CM39:CP39,CM41:CP41,CM43:CP43,CM45:CP45,CM47:CP47,CM49:CP49,CM51:CP51,CM53:CP53,CM55:CP55,CM57:CP57,CM59:CP59)</f>
-        <v>0</v>
-      </c>
-      <c r="CN64" s="36"/>
-      <c r="CO64" s="36"/>
-      <c r="CP64" s="37"/>
-      <c r="CQ64" s="32">
-        <f t="shared" ref="CQ64:CQ65" si="41">SUM(CQ7:CT7,CQ9:CT9,CQ11:CT11,CQ13:CT13,CQ15:CT15,CQ17:CT17,CQ19:CT19,CQ21:CT21,CQ23:CT23,CQ25:CT25,CQ28:CT28,CQ30:CT30,CQ32:CT32,CQ34:CT34,CQ37:CT37,CQ39:CT39,CQ41:CT41,CQ43:CT43,CQ45:CT45,CQ47:CT47,CQ49:CT49,CQ51:CT51,CQ53:CT53,CQ55:CT55,CQ57:CT57,CQ59:CT59)</f>
-        <v>0</v>
-      </c>
-      <c r="CR64" s="36"/>
-      <c r="CS64" s="36"/>
-      <c r="CT64" s="37"/>
+        <v>1.5</v>
+      </c>
+      <c r="BL64" s="53"/>
+      <c r="BM64" s="53"/>
+      <c r="BN64" s="54"/>
+      <c r="BO64" s="52">
+        <f>SUM(BO7:BR7,BO9:BR9,BO11:BR11,BO13:BR13,BO15:BR15,BO17:BR17,BO19:BR19,BO21:BR21,BO23:BR23,BO25:BR25,BO28:BR28,BO30:BR30,BO32:BR32,BO34:BR34,BO37:BR37,BO39:BR39,BO41:BR41,BO43:BR43,BO45:BR45,BO47:BR47,BO49:BR49,BO51:BR51,BO53:BR53,BO55:BR55,BO57:BR57,BO59:BR59)</f>
+        <v>2.5</v>
+      </c>
+      <c r="BP64" s="53"/>
+      <c r="BQ64" s="53"/>
+      <c r="BR64" s="54"/>
+      <c r="BS64" s="52">
+        <f t="shared" ref="BS64:BS65" si="34">SUM(BS7:BV7,BS9:BV9,BS11:BV11,BS13:BV13,BS15:BV15,BS17:BV17,BS19:BV19,BS21:BV21,BS23:BV23,BS25:BV25,BS28:BV28,BS30:BV30,BS32:BV32,BS34:BV34,BS37:BV37,BS39:BV39,BS41:BV41,BS43:BV43,BS45:BV45,BS47:BV47,BS49:BV49,BS51:BV51,BS53:BV53,BS55:BV55,BS57:BV57,BS59:BV59)</f>
+        <v>2.5</v>
+      </c>
+      <c r="BT64" s="53"/>
+      <c r="BU64" s="53"/>
+      <c r="BV64" s="54"/>
+      <c r="BW64" s="52">
+        <f t="shared" ref="BW64:BW65" si="35">SUM(BW7:BZ7,BW9:BZ9,BW11:BZ11,BW13:BZ13,BW15:BZ15,BW17:BZ17,BW19:BZ19,BW21:BZ21,BW23:BZ23,BW25:BZ25,BW28:BZ28,BW30:BZ30,BW32:BZ32,BW34:BZ34,BW37:BZ37,BW39:BZ39,BW41:BZ41,BW43:BZ43,BW45:BZ45,BW47:BZ47,BW49:BZ49,BW51:BZ51,BW53:BZ53,BW55:BZ55,BW57:BZ57,BW59:BZ59)</f>
+        <v>1.5</v>
+      </c>
+      <c r="BX64" s="53"/>
+      <c r="BY64" s="53"/>
+      <c r="BZ64" s="54"/>
+      <c r="CA64" s="52">
+        <f t="shared" ref="CA64:CA65" si="36">SUM(CA7:CD7,CA9:CD9,CA11:CD11,CA13:CD13,CA15:CD15,CA17:CD17,CA19:CD19,CA21:CD21,CA23:CD23,CA25:CD25,CA28:CD28,CA30:CD30,CA32:CD32,CA34:CD34,CA37:CD37,CA39:CD39,CA41:CD41,CA43:CD43,CA45:CD45,CA47:CD47,CA49:CD49,CA51:CD51,CA53:CD53,CA55:CD55,CA57:CD57,CA59:CD59)</f>
+        <v>2.5</v>
+      </c>
+      <c r="CB64" s="53"/>
+      <c r="CC64" s="53"/>
+      <c r="CD64" s="54"/>
+      <c r="CE64" s="52">
+        <f t="shared" ref="CE64:CE65" si="37">SUM(CE7:CH7,CE9:CH9,CE11:CH11,CE13:CH13,CE15:CH15,CE17:CH17,CE19:CH19,CE21:CH21,CE23:CH23,CE25:CH25,CE28:CH28,CE30:CH30,CE32:CH32,CE34:CH34,CE37:CH37,CE39:CH39,CE41:CH41,CE43:CH43,CE45:CH45,CE47:CH47,CE49:CH49,CE51:CH51,CE53:CH53,CE55:CH55,CE57:CH57,CE59:CH59)</f>
+        <v>2.5</v>
+      </c>
+      <c r="CF64" s="53"/>
+      <c r="CG64" s="53"/>
+      <c r="CH64" s="54"/>
+      <c r="CI64" s="52">
+        <f t="shared" ref="CI64:CI65" si="38">SUM(CI7:CL7,CI9:CL9,CI11:CL11,CI13:CL13,CI15:CL15,CI17:CL17,CI19:CL19,CI21:CL21,CI23:CL23,CI25:CL25,CI28:CL28,CI30:CL30,CI32:CL32,CI34:CL34,CI37:CL37,CI39:CL39,CI41:CL41,CI43:CL43,CI45:CL45,CI47:CL47,CI49:CL49,CI51:CL51,CI53:CL53,CI55:CL55,CI57:CL57,CI59:CL59)</f>
+        <v>1.5</v>
+      </c>
+      <c r="CJ64" s="53"/>
+      <c r="CK64" s="53"/>
+      <c r="CL64" s="54"/>
+      <c r="CM64" s="52">
+        <f t="shared" ref="CM64:CM65" si="39">SUM(CM7:CP7,CM9:CP9,CM11:CP11,CM13:CP13,CM15:CP15,CM17:CP17,CM19:CP19,CM21:CP21,CM23:CP23,CM25:CP25,CM28:CP28,CM30:CP30,CM32:CP32,CM34:CP34,CM37:CP37,CM39:CP39,CM41:CP41,CM43:CP43,CM45:CP45,CM47:CP47,CM49:CP49,CM51:CP51,CM53:CP53,CM55:CP55,CM57:CP57,CM59:CP59)</f>
+        <v>3</v>
+      </c>
+      <c r="CN64" s="53"/>
+      <c r="CO64" s="53"/>
+      <c r="CP64" s="54"/>
+      <c r="CQ64" s="52">
+        <f t="shared" ref="CQ64:CQ65" si="40">SUM(CQ7:CT7,CQ9:CT9,CQ11:CT11,CQ13:CT13,CQ15:CT15,CQ17:CT17,CQ19:CT19,CQ21:CT21,CQ23:CT23,CQ25:CT25,CQ28:CT28,CQ30:CT30,CQ32:CT32,CQ34:CT34,CQ37:CT37,CQ39:CT39,CQ41:CT41,CQ43:CT43,CQ45:CT45,CQ47:CT47,CQ49:CT49,CQ51:CT51,CQ53:CT53,CQ55:CT55,CQ57:CT57,CQ59:CT59)</f>
+        <v>1.5</v>
+      </c>
+      <c r="CR64" s="53"/>
+      <c r="CS64" s="53"/>
+      <c r="CT64" s="54"/>
     </row>
     <row r="65" spans="3:98" x14ac:dyDescent="0.35">
       <c r="C65" s="6" t="s">
@@ -7295,209 +7367,419 @@
       <c r="D65" s="6"/>
       <c r="E65" s="7">
         <f>SUM(E7:E60)</f>
-        <v>21</v>
+        <v>22.5</v>
       </c>
       <c r="F65" s="8"/>
-      <c r="G65" s="32">
+      <c r="G65" s="52">
         <f>SUM(G8:J8,G10:J10,G12:J12,G14:J14,G16:J16,G18:J18,G20:J20,G22:J22,G24:J24,G26:J26,G29:J29,G31:J31,G33:J33,G35:J35,G38:J38,G40:J40,G42:J42,G44:J44,G46:J46,G48:J48,G50:J50,G52:J52,G54:J54,G56:J56,G58:J58,G60:J60)</f>
         <v>4.5</v>
       </c>
-      <c r="H65" s="36"/>
-      <c r="I65" s="36"/>
-      <c r="J65" s="37"/>
-      <c r="K65" s="32">
+      <c r="H65" s="53"/>
+      <c r="I65" s="53"/>
+      <c r="J65" s="54"/>
+      <c r="K65" s="52">
         <f t="shared" si="20"/>
         <v>4.5</v>
       </c>
-      <c r="L65" s="36"/>
-      <c r="M65" s="36"/>
-      <c r="N65" s="37"/>
-      <c r="O65" s="32">
+      <c r="L65" s="53"/>
+      <c r="M65" s="53"/>
+      <c r="N65" s="54"/>
+      <c r="O65" s="52">
         <f t="shared" si="21"/>
         <v>4.5</v>
       </c>
-      <c r="P65" s="36"/>
-      <c r="Q65" s="36"/>
-      <c r="R65" s="37"/>
-      <c r="S65" s="32">
+      <c r="P65" s="53"/>
+      <c r="Q65" s="53"/>
+      <c r="R65" s="54"/>
+      <c r="S65" s="52">
         <f t="shared" si="22"/>
         <v>1.5</v>
       </c>
-      <c r="T65" s="36"/>
-      <c r="U65" s="36"/>
-      <c r="V65" s="37"/>
-      <c r="W65" s="32">
+      <c r="T65" s="53"/>
+      <c r="U65" s="53"/>
+      <c r="V65" s="54"/>
+      <c r="W65" s="52">
         <f t="shared" si="23"/>
         <v>1.5</v>
       </c>
-      <c r="X65" s="36"/>
-      <c r="Y65" s="36"/>
-      <c r="Z65" s="37"/>
-      <c r="AA65" s="32">
+      <c r="X65" s="53"/>
+      <c r="Y65" s="53"/>
+      <c r="Z65" s="54"/>
+      <c r="AA65" s="52">
         <f t="shared" si="24"/>
         <v>1.5</v>
       </c>
-      <c r="AB65" s="36"/>
-      <c r="AC65" s="36"/>
-      <c r="AD65" s="37"/>
-      <c r="AE65" s="32">
+      <c r="AB65" s="53"/>
+      <c r="AC65" s="53"/>
+      <c r="AD65" s="54"/>
+      <c r="AE65" s="52">
         <f t="shared" si="25"/>
         <v>1.5</v>
       </c>
-      <c r="AF65" s="36"/>
-      <c r="AG65" s="36"/>
-      <c r="AH65" s="37"/>
-      <c r="AI65" s="32">
+      <c r="AF65" s="53"/>
+      <c r="AG65" s="53"/>
+      <c r="AH65" s="54"/>
+      <c r="AI65" s="52">
         <f t="shared" si="26"/>
         <v>1.5</v>
       </c>
-      <c r="AJ65" s="36"/>
-      <c r="AK65" s="36"/>
-      <c r="AL65" s="37"/>
-      <c r="AM65" s="32">
+      <c r="AJ65" s="53"/>
+      <c r="AK65" s="53"/>
+      <c r="AL65" s="54"/>
+      <c r="AM65" s="52">
         <f t="shared" si="27"/>
-        <v>0</v>
-      </c>
-      <c r="AN65" s="36"/>
-      <c r="AO65" s="36"/>
-      <c r="AP65" s="37"/>
-      <c r="AQ65" s="32">
+        <v>1.5</v>
+      </c>
+      <c r="AN65" s="53"/>
+      <c r="AO65" s="53"/>
+      <c r="AP65" s="54"/>
+      <c r="AQ65" s="52">
         <f t="shared" si="28"/>
         <v>0</v>
       </c>
-      <c r="AR65" s="36"/>
-      <c r="AS65" s="36"/>
-      <c r="AT65" s="37"/>
-      <c r="AU65" s="32">
+      <c r="AR65" s="53"/>
+      <c r="AS65" s="53"/>
+      <c r="AT65" s="54"/>
+      <c r="AU65" s="52">
         <f t="shared" si="29"/>
         <v>0</v>
       </c>
-      <c r="AV65" s="36"/>
-      <c r="AW65" s="36"/>
-      <c r="AX65" s="37"/>
-      <c r="AY65" s="32">
+      <c r="AV65" s="53"/>
+      <c r="AW65" s="53"/>
+      <c r="AX65" s="54"/>
+      <c r="AY65" s="52">
         <f t="shared" si="30"/>
         <v>0</v>
       </c>
-      <c r="AZ65" s="36"/>
-      <c r="BA65" s="36"/>
-      <c r="BB65" s="37"/>
-      <c r="BC65" s="32">
+      <c r="AZ65" s="53"/>
+      <c r="BA65" s="53"/>
+      <c r="BB65" s="54"/>
+      <c r="BC65" s="52">
         <f t="shared" si="31"/>
         <v>0</v>
       </c>
-      <c r="BD65" s="36"/>
-      <c r="BE65" s="36"/>
-      <c r="BF65" s="37"/>
-      <c r="BG65" s="32">
+      <c r="BD65" s="53"/>
+      <c r="BE65" s="53"/>
+      <c r="BF65" s="54"/>
+      <c r="BG65" s="52">
         <f t="shared" si="32"/>
         <v>0</v>
       </c>
-      <c r="BH65" s="36"/>
-      <c r="BI65" s="36"/>
-      <c r="BJ65" s="37"/>
-      <c r="BK65" s="32">
+      <c r="BH65" s="53"/>
+      <c r="BI65" s="53"/>
+      <c r="BJ65" s="54"/>
+      <c r="BK65" s="52">
         <f t="shared" si="33"/>
         <v>0</v>
       </c>
-      <c r="BL65" s="36"/>
-      <c r="BM65" s="36"/>
-      <c r="BN65" s="37"/>
-      <c r="BO65" s="32">
+      <c r="BL65" s="53"/>
+      <c r="BM65" s="53"/>
+      <c r="BN65" s="54"/>
+      <c r="BO65" s="52">
+        <f t="shared" ref="BO65" si="41">SUM(BO8:BR8,BO10:BR10,BO12:BR12,BO14:BR14,BO16:BR16,BO18:BR18,BO20:BR20,BO22:BR22,BO24:BR24,BO26:BR26,BO29:BR29,BO31:BR31,BO33:BR33,BO35:BR35,BO38:BR38,BO40:BR40,BO42:BR42,BO44:BR44,BO46:BR46,BO48:BR48,BO50:BR50,BO52:BR52,BO54:BR54,BO56:BR56,BO58:BR58,BO60:BR60)</f>
+        <v>0</v>
+      </c>
+      <c r="BP65" s="53"/>
+      <c r="BQ65" s="53"/>
+      <c r="BR65" s="54"/>
+      <c r="BS65" s="52">
         <f t="shared" si="34"/>
         <v>0</v>
       </c>
-      <c r="BP65" s="36"/>
-      <c r="BQ65" s="36"/>
-      <c r="BR65" s="37"/>
-      <c r="BS65" s="32">
+      <c r="BT65" s="53"/>
+      <c r="BU65" s="53"/>
+      <c r="BV65" s="54"/>
+      <c r="BW65" s="52">
         <f t="shared" si="35"/>
         <v>0</v>
       </c>
-      <c r="BT65" s="36"/>
-      <c r="BU65" s="36"/>
-      <c r="BV65" s="37"/>
-      <c r="BW65" s="32">
+      <c r="BX65" s="53"/>
+      <c r="BY65" s="53"/>
+      <c r="BZ65" s="54"/>
+      <c r="CA65" s="52">
         <f t="shared" si="36"/>
         <v>0</v>
       </c>
-      <c r="BX65" s="36"/>
-      <c r="BY65" s="36"/>
-      <c r="BZ65" s="37"/>
-      <c r="CA65" s="32">
+      <c r="CB65" s="53"/>
+      <c r="CC65" s="53"/>
+      <c r="CD65" s="54"/>
+      <c r="CE65" s="52">
         <f t="shared" si="37"/>
         <v>0</v>
       </c>
-      <c r="CB65" s="36"/>
-      <c r="CC65" s="36"/>
-      <c r="CD65" s="37"/>
-      <c r="CE65" s="32">
+      <c r="CF65" s="53"/>
+      <c r="CG65" s="53"/>
+      <c r="CH65" s="54"/>
+      <c r="CI65" s="52">
         <f t="shared" si="38"/>
         <v>0</v>
       </c>
-      <c r="CF65" s="36"/>
-      <c r="CG65" s="36"/>
-      <c r="CH65" s="37"/>
-      <c r="CI65" s="32">
+      <c r="CJ65" s="53"/>
+      <c r="CK65" s="53"/>
+      <c r="CL65" s="54"/>
+      <c r="CM65" s="52">
         <f t="shared" si="39"/>
         <v>0</v>
       </c>
-      <c r="CJ65" s="36"/>
-      <c r="CK65" s="36"/>
-      <c r="CL65" s="37"/>
-      <c r="CM65" s="32">
+      <c r="CN65" s="53"/>
+      <c r="CO65" s="53"/>
+      <c r="CP65" s="54"/>
+      <c r="CQ65" s="52">
         <f t="shared" si="40"/>
         <v>0</v>
       </c>
-      <c r="CN65" s="36"/>
-      <c r="CO65" s="36"/>
-      <c r="CP65" s="37"/>
-      <c r="CQ65" s="32">
-        <f t="shared" si="41"/>
-        <v>0</v>
-      </c>
-      <c r="CR65" s="36"/>
-      <c r="CS65" s="36"/>
-      <c r="CT65" s="37"/>
+      <c r="CR65" s="53"/>
+      <c r="CS65" s="53"/>
+      <c r="CT65" s="54"/>
     </row>
     <row r="66" spans="3:98" x14ac:dyDescent="0.35">
       <c r="C66" s="6" t="s">
         <v>13</v>
       </c>
-      <c r="D66" s="38">
+      <c r="D66" s="55">
         <f>D64-E65</f>
-        <v>3</v>
-      </c>
-      <c r="E66" s="39"/>
+        <v>27.5</v>
+      </c>
+      <c r="E66" s="56"/>
     </row>
   </sheetData>
-  <mergeCells count="251">
-    <mergeCell ref="AQ25:AR25"/>
-    <mergeCell ref="AQ26:AR26"/>
-    <mergeCell ref="AA4:AD4"/>
-    <mergeCell ref="AE4:AH4"/>
-    <mergeCell ref="CI4:CL4"/>
-    <mergeCell ref="Q5:R5"/>
-    <mergeCell ref="S5:T5"/>
-    <mergeCell ref="U5:V5"/>
-    <mergeCell ref="W5:X5"/>
-    <mergeCell ref="D2:D5"/>
-    <mergeCell ref="E2:E5"/>
-    <mergeCell ref="F2:F5"/>
-    <mergeCell ref="G5:H5"/>
-    <mergeCell ref="I5:J5"/>
-    <mergeCell ref="K5:L5"/>
-    <mergeCell ref="CE4:CH4"/>
-    <mergeCell ref="CE5:CF5"/>
-    <mergeCell ref="CG5:CH5"/>
-    <mergeCell ref="CA4:CD4"/>
-    <mergeCell ref="CA5:CB5"/>
-    <mergeCell ref="CC5:CD5"/>
-    <mergeCell ref="AU4:AX4"/>
-    <mergeCell ref="AU5:AV5"/>
-    <mergeCell ref="AW5:AX5"/>
-    <mergeCell ref="AI4:AL4"/>
-    <mergeCell ref="AI5:AJ5"/>
+  <mergeCells count="308">
+    <mergeCell ref="AM18:AN18"/>
+    <mergeCell ref="CA54:CB54"/>
+    <mergeCell ref="CA53:CB53"/>
+    <mergeCell ref="CO58:CP58"/>
+    <mergeCell ref="CO57:CP57"/>
+    <mergeCell ref="CO60:CP60"/>
+    <mergeCell ref="CO59:CP59"/>
+    <mergeCell ref="CG56:CH56"/>
+    <mergeCell ref="CG55:CH55"/>
+    <mergeCell ref="CC54:CD54"/>
+    <mergeCell ref="CC53:CD53"/>
+    <mergeCell ref="CQ60:CR60"/>
+    <mergeCell ref="CQ59:CR59"/>
+    <mergeCell ref="CM58:CN58"/>
+    <mergeCell ref="CM57:CN57"/>
+    <mergeCell ref="CI56:CJ56"/>
+    <mergeCell ref="CI55:CJ55"/>
+    <mergeCell ref="CE56:CF56"/>
+    <mergeCell ref="CE55:CF55"/>
+    <mergeCell ref="CE54:CF54"/>
+    <mergeCell ref="BW52:BX52"/>
+    <mergeCell ref="BW51:BX51"/>
+    <mergeCell ref="BS52:BT52"/>
+    <mergeCell ref="BS51:BT51"/>
+    <mergeCell ref="BS50:BT50"/>
+    <mergeCell ref="BS49:BT49"/>
+    <mergeCell ref="BO50:BP50"/>
+    <mergeCell ref="BO49:BP49"/>
+    <mergeCell ref="BO48:BP48"/>
+    <mergeCell ref="BU52:BV52"/>
+    <mergeCell ref="BU51:BV51"/>
+    <mergeCell ref="BQ50:BR50"/>
+    <mergeCell ref="BQ49:BR49"/>
+    <mergeCell ref="AU33:AV33"/>
+    <mergeCell ref="AU32:AV32"/>
+    <mergeCell ref="AU31:AV31"/>
+    <mergeCell ref="AU30:AV30"/>
+    <mergeCell ref="AU28:AV28"/>
+    <mergeCell ref="AU29:AV29"/>
+    <mergeCell ref="BE44:BF44"/>
+    <mergeCell ref="BE43:BF43"/>
+    <mergeCell ref="BC44:BD44"/>
+    <mergeCell ref="BC43:BD43"/>
+    <mergeCell ref="BC41:BD41"/>
+    <mergeCell ref="BC42:BD42"/>
+    <mergeCell ref="BC40:BD40"/>
+    <mergeCell ref="BC39:BD39"/>
+    <mergeCell ref="AY38:AZ38"/>
+    <mergeCell ref="AY37:AZ37"/>
+    <mergeCell ref="AY35:AZ35"/>
+    <mergeCell ref="AY34:AZ34"/>
+    <mergeCell ref="AY5:AZ5"/>
+    <mergeCell ref="BA5:BB5"/>
+    <mergeCell ref="AK5:AL5"/>
+    <mergeCell ref="F13:F14"/>
+    <mergeCell ref="D15:D16"/>
+    <mergeCell ref="E15:E16"/>
+    <mergeCell ref="F15:F16"/>
+    <mergeCell ref="C13:C14"/>
+    <mergeCell ref="C15:C16"/>
+    <mergeCell ref="AE16:AF16"/>
+    <mergeCell ref="AE15:AF15"/>
+    <mergeCell ref="AA16:AB16"/>
+    <mergeCell ref="AA15:AB15"/>
+    <mergeCell ref="W14:X14"/>
+    <mergeCell ref="W13:X13"/>
+    <mergeCell ref="S14:T14"/>
+    <mergeCell ref="S13:T13"/>
+    <mergeCell ref="AI64:AL64"/>
+    <mergeCell ref="AI17:AJ17"/>
+    <mergeCell ref="AI18:AJ18"/>
+    <mergeCell ref="G7:H7"/>
+    <mergeCell ref="G8:H8"/>
+    <mergeCell ref="O12:P12"/>
+    <mergeCell ref="O11:P11"/>
+    <mergeCell ref="K12:L12"/>
+    <mergeCell ref="K11:L11"/>
+    <mergeCell ref="K10:L10"/>
+    <mergeCell ref="K9:L9"/>
+    <mergeCell ref="G10:H10"/>
+    <mergeCell ref="G9:H9"/>
+    <mergeCell ref="BC4:BF4"/>
+    <mergeCell ref="BC5:BD5"/>
+    <mergeCell ref="BE5:BF5"/>
+    <mergeCell ref="BC64:BF64"/>
+    <mergeCell ref="BC65:BF65"/>
+    <mergeCell ref="BO4:BR4"/>
+    <mergeCell ref="BO5:BP5"/>
+    <mergeCell ref="BQ5:BR5"/>
+    <mergeCell ref="BO64:BR64"/>
+    <mergeCell ref="BO65:BR65"/>
+    <mergeCell ref="BK4:BN4"/>
+    <mergeCell ref="BK5:BL5"/>
+    <mergeCell ref="BM5:BN5"/>
+    <mergeCell ref="BK64:BN64"/>
+    <mergeCell ref="BK65:BN65"/>
+    <mergeCell ref="BO47:BP47"/>
+    <mergeCell ref="BK48:BL48"/>
+    <mergeCell ref="BK47:BL47"/>
+    <mergeCell ref="BG46:BH46"/>
+    <mergeCell ref="BG45:BH45"/>
+    <mergeCell ref="CM65:CP65"/>
+    <mergeCell ref="CQ65:CT65"/>
+    <mergeCell ref="D66:E66"/>
+    <mergeCell ref="AE64:AH64"/>
+    <mergeCell ref="CI64:CL64"/>
+    <mergeCell ref="CM64:CP64"/>
+    <mergeCell ref="CQ64:CT64"/>
+    <mergeCell ref="G65:J65"/>
+    <mergeCell ref="K65:N65"/>
+    <mergeCell ref="O65:R65"/>
+    <mergeCell ref="S65:V65"/>
+    <mergeCell ref="W65:Z65"/>
+    <mergeCell ref="AA65:AD65"/>
+    <mergeCell ref="G64:J64"/>
+    <mergeCell ref="K64:N64"/>
+    <mergeCell ref="O64:R64"/>
+    <mergeCell ref="S64:V64"/>
+    <mergeCell ref="W64:Z64"/>
+    <mergeCell ref="AA64:AD64"/>
+    <mergeCell ref="CE64:CH64"/>
+    <mergeCell ref="CE65:CH65"/>
+    <mergeCell ref="CA64:CD64"/>
+    <mergeCell ref="CA65:CD65"/>
+    <mergeCell ref="BW64:BZ64"/>
+    <mergeCell ref="F59:F60"/>
+    <mergeCell ref="D53:D54"/>
+    <mergeCell ref="E53:E54"/>
+    <mergeCell ref="F53:F54"/>
+    <mergeCell ref="D55:D56"/>
+    <mergeCell ref="E55:E56"/>
+    <mergeCell ref="F55:F56"/>
+    <mergeCell ref="AE65:AH65"/>
+    <mergeCell ref="CI65:CL65"/>
+    <mergeCell ref="BW65:BZ65"/>
+    <mergeCell ref="BS64:BV64"/>
+    <mergeCell ref="BS65:BV65"/>
+    <mergeCell ref="AU64:AX64"/>
+    <mergeCell ref="AU65:AX65"/>
+    <mergeCell ref="AQ64:AT64"/>
+    <mergeCell ref="AQ65:AT65"/>
+    <mergeCell ref="AM64:AP64"/>
+    <mergeCell ref="AM65:AP65"/>
+    <mergeCell ref="BG64:BJ64"/>
+    <mergeCell ref="BG65:BJ65"/>
+    <mergeCell ref="AY64:BB64"/>
+    <mergeCell ref="AY65:BB65"/>
+    <mergeCell ref="AI65:AL65"/>
+    <mergeCell ref="CE53:CF53"/>
+    <mergeCell ref="C59:C60"/>
+    <mergeCell ref="C37:C38"/>
+    <mergeCell ref="C39:C40"/>
+    <mergeCell ref="C41:C42"/>
+    <mergeCell ref="C43:C44"/>
+    <mergeCell ref="C45:C46"/>
+    <mergeCell ref="C47:C48"/>
+    <mergeCell ref="D41:D42"/>
+    <mergeCell ref="E41:E42"/>
+    <mergeCell ref="D43:D44"/>
+    <mergeCell ref="E43:E44"/>
+    <mergeCell ref="D37:D38"/>
+    <mergeCell ref="E37:E38"/>
+    <mergeCell ref="D39:D40"/>
+    <mergeCell ref="E39:E40"/>
+    <mergeCell ref="D49:D50"/>
+    <mergeCell ref="E49:E50"/>
+    <mergeCell ref="D51:D52"/>
+    <mergeCell ref="E51:E52"/>
+    <mergeCell ref="D45:D46"/>
+    <mergeCell ref="D59:D60"/>
+    <mergeCell ref="E59:E60"/>
+    <mergeCell ref="C49:C50"/>
+    <mergeCell ref="C51:C52"/>
+    <mergeCell ref="C53:C54"/>
+    <mergeCell ref="C55:C56"/>
+    <mergeCell ref="C57:C58"/>
+    <mergeCell ref="F41:F42"/>
+    <mergeCell ref="F43:F44"/>
+    <mergeCell ref="F37:F38"/>
+    <mergeCell ref="F39:F40"/>
+    <mergeCell ref="F49:F50"/>
+    <mergeCell ref="F51:F52"/>
+    <mergeCell ref="F45:F46"/>
+    <mergeCell ref="F47:F48"/>
+    <mergeCell ref="E57:E58"/>
+    <mergeCell ref="F57:F58"/>
+    <mergeCell ref="E45:E46"/>
+    <mergeCell ref="D47:D48"/>
+    <mergeCell ref="E47:E48"/>
+    <mergeCell ref="D57:D58"/>
+    <mergeCell ref="C28:C29"/>
+    <mergeCell ref="C30:C31"/>
+    <mergeCell ref="C32:C33"/>
+    <mergeCell ref="C34:C35"/>
+    <mergeCell ref="D34:D35"/>
+    <mergeCell ref="E34:E35"/>
+    <mergeCell ref="D28:D29"/>
+    <mergeCell ref="E28:E29"/>
+    <mergeCell ref="F28:F29"/>
+    <mergeCell ref="D30:D31"/>
+    <mergeCell ref="E30:E31"/>
+    <mergeCell ref="F30:F31"/>
+    <mergeCell ref="D32:D33"/>
+    <mergeCell ref="E32:E33"/>
+    <mergeCell ref="F32:F33"/>
+    <mergeCell ref="F34:F35"/>
+    <mergeCell ref="F25:F26"/>
+    <mergeCell ref="F9:F10"/>
+    <mergeCell ref="F11:F12"/>
+    <mergeCell ref="D23:D24"/>
+    <mergeCell ref="E23:E24"/>
+    <mergeCell ref="F23:F24"/>
+    <mergeCell ref="D19:D20"/>
+    <mergeCell ref="E19:E20"/>
+    <mergeCell ref="F19:F20"/>
+    <mergeCell ref="D21:D22"/>
+    <mergeCell ref="E21:E22"/>
+    <mergeCell ref="F21:F22"/>
+    <mergeCell ref="D17:D18"/>
+    <mergeCell ref="E17:E18"/>
+    <mergeCell ref="F17:F18"/>
+    <mergeCell ref="C25:C26"/>
+    <mergeCell ref="D13:D14"/>
+    <mergeCell ref="C9:C10"/>
+    <mergeCell ref="D9:D10"/>
+    <mergeCell ref="E9:E10"/>
+    <mergeCell ref="C11:C12"/>
+    <mergeCell ref="D11:D12"/>
+    <mergeCell ref="E11:E12"/>
+    <mergeCell ref="E13:E14"/>
+    <mergeCell ref="C23:C24"/>
+    <mergeCell ref="C19:C20"/>
+    <mergeCell ref="D25:D26"/>
+    <mergeCell ref="E25:E26"/>
+    <mergeCell ref="C21:C22"/>
+    <mergeCell ref="C17:C18"/>
     <mergeCell ref="CM4:CP4"/>
     <mergeCell ref="CQ4:CT4"/>
     <mergeCell ref="C7:C8"/>
@@ -7522,140 +7804,45 @@
     <mergeCell ref="CI5:CJ5"/>
     <mergeCell ref="M5:N5"/>
     <mergeCell ref="O5:P5"/>
-    <mergeCell ref="C25:C26"/>
-    <mergeCell ref="D13:D14"/>
-    <mergeCell ref="C9:C10"/>
-    <mergeCell ref="D9:D10"/>
-    <mergeCell ref="E9:E10"/>
-    <mergeCell ref="C11:C12"/>
-    <mergeCell ref="D11:D12"/>
-    <mergeCell ref="E11:E12"/>
-    <mergeCell ref="E13:E14"/>
-    <mergeCell ref="C23:C24"/>
-    <mergeCell ref="C19:C20"/>
-    <mergeCell ref="D25:D26"/>
-    <mergeCell ref="E25:E26"/>
-    <mergeCell ref="F25:F26"/>
-    <mergeCell ref="F9:F10"/>
-    <mergeCell ref="F11:F12"/>
-    <mergeCell ref="D23:D24"/>
-    <mergeCell ref="E23:E24"/>
-    <mergeCell ref="F23:F24"/>
-    <mergeCell ref="D19:D20"/>
-    <mergeCell ref="E19:E20"/>
-    <mergeCell ref="F19:F20"/>
-    <mergeCell ref="C28:C29"/>
-    <mergeCell ref="C30:C31"/>
-    <mergeCell ref="C32:C33"/>
-    <mergeCell ref="C34:C35"/>
-    <mergeCell ref="D34:D35"/>
-    <mergeCell ref="E34:E35"/>
-    <mergeCell ref="D28:D29"/>
-    <mergeCell ref="E28:E29"/>
-    <mergeCell ref="F28:F29"/>
-    <mergeCell ref="D30:D31"/>
-    <mergeCell ref="E30:E31"/>
-    <mergeCell ref="F30:F31"/>
-    <mergeCell ref="D32:D33"/>
-    <mergeCell ref="E32:E33"/>
-    <mergeCell ref="F32:F33"/>
-    <mergeCell ref="F34:F35"/>
-    <mergeCell ref="C49:C50"/>
-    <mergeCell ref="C51:C52"/>
-    <mergeCell ref="C53:C54"/>
-    <mergeCell ref="C55:C56"/>
-    <mergeCell ref="C57:C58"/>
-    <mergeCell ref="F41:F42"/>
-    <mergeCell ref="F43:F44"/>
-    <mergeCell ref="F37:F38"/>
-    <mergeCell ref="F39:F40"/>
-    <mergeCell ref="F49:F50"/>
-    <mergeCell ref="F51:F52"/>
-    <mergeCell ref="F45:F46"/>
-    <mergeCell ref="F47:F48"/>
-    <mergeCell ref="E57:E58"/>
-    <mergeCell ref="F57:F58"/>
-    <mergeCell ref="E45:E46"/>
-    <mergeCell ref="D47:D48"/>
-    <mergeCell ref="E47:E48"/>
-    <mergeCell ref="D57:D58"/>
-    <mergeCell ref="C59:C60"/>
-    <mergeCell ref="C37:C38"/>
-    <mergeCell ref="C39:C40"/>
-    <mergeCell ref="C41:C42"/>
-    <mergeCell ref="C43:C44"/>
-    <mergeCell ref="C45:C46"/>
-    <mergeCell ref="C47:C48"/>
-    <mergeCell ref="D41:D42"/>
-    <mergeCell ref="E41:E42"/>
-    <mergeCell ref="D43:D44"/>
-    <mergeCell ref="E43:E44"/>
-    <mergeCell ref="D37:D38"/>
-    <mergeCell ref="E37:E38"/>
-    <mergeCell ref="D39:D40"/>
-    <mergeCell ref="E39:E40"/>
-    <mergeCell ref="D49:D50"/>
-    <mergeCell ref="E49:E50"/>
-    <mergeCell ref="D51:D52"/>
-    <mergeCell ref="E51:E52"/>
-    <mergeCell ref="D45:D46"/>
-    <mergeCell ref="D59:D60"/>
-    <mergeCell ref="E59:E60"/>
-    <mergeCell ref="F59:F60"/>
-    <mergeCell ref="D53:D54"/>
-    <mergeCell ref="E53:E54"/>
-    <mergeCell ref="F53:F54"/>
-    <mergeCell ref="D55:D56"/>
-    <mergeCell ref="E55:E56"/>
-    <mergeCell ref="F55:F56"/>
-    <mergeCell ref="AE65:AH65"/>
-    <mergeCell ref="CI65:CL65"/>
-    <mergeCell ref="CM65:CP65"/>
-    <mergeCell ref="CQ65:CT65"/>
-    <mergeCell ref="D66:E66"/>
-    <mergeCell ref="AE64:AH64"/>
-    <mergeCell ref="CI64:CL64"/>
-    <mergeCell ref="CM64:CP64"/>
-    <mergeCell ref="CQ64:CT64"/>
-    <mergeCell ref="G65:J65"/>
-    <mergeCell ref="K65:N65"/>
-    <mergeCell ref="O65:R65"/>
-    <mergeCell ref="S65:V65"/>
-    <mergeCell ref="W65:Z65"/>
-    <mergeCell ref="AA65:AD65"/>
-    <mergeCell ref="G64:J64"/>
-    <mergeCell ref="K64:N64"/>
-    <mergeCell ref="O64:R64"/>
-    <mergeCell ref="S64:V64"/>
-    <mergeCell ref="W64:Z64"/>
-    <mergeCell ref="AA64:AD64"/>
-    <mergeCell ref="CE64:CH64"/>
-    <mergeCell ref="CE65:CH65"/>
-    <mergeCell ref="CA64:CD64"/>
-    <mergeCell ref="CA65:CD65"/>
+    <mergeCell ref="D2:D5"/>
+    <mergeCell ref="E2:E5"/>
+    <mergeCell ref="F2:F5"/>
+    <mergeCell ref="G5:H5"/>
+    <mergeCell ref="I5:J5"/>
+    <mergeCell ref="K5:L5"/>
+    <mergeCell ref="CE4:CH4"/>
+    <mergeCell ref="CE5:CF5"/>
+    <mergeCell ref="CG5:CH5"/>
+    <mergeCell ref="CA4:CD4"/>
+    <mergeCell ref="CA5:CB5"/>
+    <mergeCell ref="CC5:CD5"/>
+    <mergeCell ref="AU4:AX4"/>
+    <mergeCell ref="AU5:AV5"/>
+    <mergeCell ref="AW5:AX5"/>
+    <mergeCell ref="AI4:AL4"/>
+    <mergeCell ref="AI5:AJ5"/>
     <mergeCell ref="BW4:BZ4"/>
     <mergeCell ref="BW5:BX5"/>
     <mergeCell ref="BY5:BZ5"/>
-    <mergeCell ref="BW64:BZ64"/>
-    <mergeCell ref="BW65:BZ65"/>
     <mergeCell ref="BS4:BV4"/>
     <mergeCell ref="BS5:BT5"/>
     <mergeCell ref="BU5:BV5"/>
-    <mergeCell ref="BS64:BV64"/>
-    <mergeCell ref="BS65:BV65"/>
     <mergeCell ref="AY4:BB4"/>
-    <mergeCell ref="AU64:AX64"/>
-    <mergeCell ref="AU65:AX65"/>
+    <mergeCell ref="AQ25:AR25"/>
+    <mergeCell ref="AQ26:AR26"/>
+    <mergeCell ref="AA4:AD4"/>
+    <mergeCell ref="AE4:AH4"/>
+    <mergeCell ref="CI4:CL4"/>
+    <mergeCell ref="Q5:R5"/>
+    <mergeCell ref="S5:T5"/>
+    <mergeCell ref="U5:V5"/>
+    <mergeCell ref="W5:X5"/>
     <mergeCell ref="AQ4:AT4"/>
     <mergeCell ref="AQ5:AR5"/>
     <mergeCell ref="AS5:AT5"/>
-    <mergeCell ref="AQ64:AT64"/>
-    <mergeCell ref="AQ65:AT65"/>
     <mergeCell ref="AM4:AP4"/>
     <mergeCell ref="AM5:AN5"/>
     <mergeCell ref="AO5:AP5"/>
-    <mergeCell ref="AM64:AP64"/>
-    <mergeCell ref="AM65:AP65"/>
     <mergeCell ref="AM19:AN19"/>
     <mergeCell ref="AM20:AN20"/>
     <mergeCell ref="AM21:AN21"/>
@@ -7665,67 +7852,9 @@
     <mergeCell ref="BG4:BJ4"/>
     <mergeCell ref="BG5:BH5"/>
     <mergeCell ref="BI5:BJ5"/>
-    <mergeCell ref="BG64:BJ64"/>
-    <mergeCell ref="BG65:BJ65"/>
-    <mergeCell ref="BC4:BF4"/>
-    <mergeCell ref="BC5:BD5"/>
-    <mergeCell ref="BE5:BF5"/>
-    <mergeCell ref="BC64:BF64"/>
-    <mergeCell ref="BC65:BF65"/>
-    <mergeCell ref="BO4:BR4"/>
-    <mergeCell ref="BO5:BP5"/>
-    <mergeCell ref="BQ5:BR5"/>
-    <mergeCell ref="BO64:BR64"/>
-    <mergeCell ref="BO65:BR65"/>
-    <mergeCell ref="BK4:BN4"/>
-    <mergeCell ref="BK5:BL5"/>
-    <mergeCell ref="BM5:BN5"/>
-    <mergeCell ref="BK64:BN64"/>
-    <mergeCell ref="BK65:BN65"/>
-    <mergeCell ref="AY64:BB64"/>
-    <mergeCell ref="AY65:BB65"/>
-    <mergeCell ref="G7:H7"/>
-    <mergeCell ref="G8:H8"/>
-    <mergeCell ref="O12:P12"/>
-    <mergeCell ref="O11:P11"/>
-    <mergeCell ref="K12:L12"/>
-    <mergeCell ref="K11:L11"/>
-    <mergeCell ref="K10:L10"/>
-    <mergeCell ref="K9:L9"/>
-    <mergeCell ref="G10:H10"/>
-    <mergeCell ref="G9:H9"/>
-    <mergeCell ref="AE16:AF16"/>
-    <mergeCell ref="AE15:AF15"/>
-    <mergeCell ref="AA16:AB16"/>
-    <mergeCell ref="AA15:AB15"/>
-    <mergeCell ref="W14:X14"/>
-    <mergeCell ref="W13:X13"/>
-    <mergeCell ref="S14:T14"/>
-    <mergeCell ref="S13:T13"/>
-    <mergeCell ref="AI64:AL64"/>
-    <mergeCell ref="AI65:AL65"/>
-    <mergeCell ref="C21:C22"/>
-    <mergeCell ref="D21:D22"/>
-    <mergeCell ref="E21:E22"/>
-    <mergeCell ref="F21:F22"/>
-    <mergeCell ref="AY5:AZ5"/>
-    <mergeCell ref="BA5:BB5"/>
-    <mergeCell ref="AK5:AL5"/>
-    <mergeCell ref="F13:F14"/>
-    <mergeCell ref="D15:D16"/>
-    <mergeCell ref="E15:E16"/>
-    <mergeCell ref="F15:F16"/>
-    <mergeCell ref="C13:C14"/>
-    <mergeCell ref="C15:C16"/>
-    <mergeCell ref="C17:C18"/>
-    <mergeCell ref="D17:D18"/>
-    <mergeCell ref="E17:E18"/>
-    <mergeCell ref="F17:F18"/>
-    <mergeCell ref="AI17:AJ17"/>
-    <mergeCell ref="AI18:AJ18"/>
   </mergeCells>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" fitToWidth="0" orientation="landscape" r:id="rId1"/>
+  <pageMargins left="0.25" right="0.25" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" scale="52" orientation="landscape" r:id="rId1"/>
   <ignoredErrors>
     <ignoredError sqref="CR4:CT4 CN4:CP4 CJ4:CL4 AF4:AH4 AB4:AD4 T4:V4 P4:R4 L4:N4 X4:Z4" twoDigitTextYear="1"/>
     <ignoredError sqref="H64:J64" formulaRange="1"/>

</xml_diff>